<commit_message>
Rewrite 0.04: II_Windows UI - Recreated UI for Patient Editor - Added icons in layout, optimized layout
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Desktop\infirmary-integrated\II_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>LoadSimulation</t>
   </si>
@@ -174,6 +174,30 @@
   </si>
   <si>
     <t>CardiacMonitor</t>
+  </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>Ventilator</t>
+  </si>
+  <si>
+    <t>IABP</t>
+  </si>
+  <si>
+    <t>Defibrillator</t>
+  </si>
+  <si>
+    <t>12LeadECG</t>
+  </si>
+  <si>
+    <t>IVPump</t>
+  </si>
+  <si>
+    <t>LabResults</t>
+  </si>
+  <si>
+    <t>Cardiotocograph</t>
   </si>
 </sst>
 </file>
@@ -500,11 +524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A31" sqref="A31"/>
+      <selection pane="topRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,61 +705,101 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rewrite 0.06: II_Windows, WPF... - WPF: Reimplemented start-up args[] input - WPF: Reimplemented menuitem shortcut keys
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -26,21 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
-    <t>LoadSimulation</t>
-  </si>
-  <si>
-    <t>SaveSimulation</t>
-  </si>
-  <si>
-    <t>ExitProgram</t>
-  </si>
-  <si>
-    <t>Help</t>
-  </si>
-  <si>
-    <t>AboutProgram</t>
-  </si>
-  <si>
     <t>HeartRate</t>
   </si>
   <si>
@@ -98,42 +83,6 @@
     <t>ResetParameters</t>
   </si>
   <si>
-    <t>DeviceOptions</t>
-  </si>
-  <si>
-    <t>PauseDevice</t>
-  </si>
-  <si>
-    <t>NumericRowAmounts</t>
-  </si>
-  <si>
-    <t>TracingRowAmounts</t>
-  </si>
-  <si>
-    <t>FontSize</t>
-  </si>
-  <si>
-    <t>ColorScheme</t>
-  </si>
-  <si>
-    <t>ToggleFullscreen</t>
-  </si>
-  <si>
-    <t>CloseDevice</t>
-  </si>
-  <si>
-    <t>PatientOptions</t>
-  </si>
-  <si>
-    <t>NewPatient</t>
-  </si>
-  <si>
-    <t>EditPatient</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>Key</t>
   </si>
   <si>
@@ -198,6 +147,57 @@
   </si>
   <si>
     <t>Cardiotocograph</t>
+  </si>
+  <si>
+    <t>MenuDeviceOptions</t>
+  </si>
+  <si>
+    <t>MenuNumericRowAmounts</t>
+  </si>
+  <si>
+    <t>MenuPauseDevice</t>
+  </si>
+  <si>
+    <t>MenuTracingRowAmounts</t>
+  </si>
+  <si>
+    <t>MenuFontSize</t>
+  </si>
+  <si>
+    <t>MenuColorScheme</t>
+  </si>
+  <si>
+    <t>MenuToggleFullscreen</t>
+  </si>
+  <si>
+    <t>MenuCloseDevice</t>
+  </si>
+  <si>
+    <t>MenuPatientOptions</t>
+  </si>
+  <si>
+    <t>MenuNewPatient</t>
+  </si>
+  <si>
+    <t>MenuEditPatient</t>
+  </si>
+  <si>
+    <t>MenuFile</t>
+  </si>
+  <si>
+    <t>MenuLoadSimulation</t>
+  </si>
+  <si>
+    <t>MenuSaveSimulation</t>
+  </si>
+  <si>
+    <t>MenuExitProgram</t>
+  </si>
+  <si>
+    <t>MenuHelp</t>
+  </si>
+  <si>
+    <t>MenuAboutProgram</t>
   </si>
 </sst>
 </file>
@@ -524,283 +524,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A37" sqref="A37"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V 0.9 (WPF, Localization, 12 Lead ECG) * Cross-platform re-write complete (merging "rewrite" branch to "master")   - Windows interface rewritten in WPF   - Localization support added throughout program - Re-write finished   - Cardiac Monitor controls layout polished   - Cardiac Monitor controls context menus re-implemented - DeviceECG (12 Lead ECG) implemented   - Control.ECGTracing utilized as less dynamic version of Control.MonitorTracing
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="899">
   <si>
     <t>Temperature</t>
   </si>
@@ -1490,9 +1490,6 @@
     <t>NUMERIC:CVP</t>
   </si>
   <si>
-    <t>NUMERIC:PAP</t>
-  </si>
-  <si>
     <t>Electrocardiograph (ECG) Lead I</t>
   </si>
   <si>
@@ -2057,42 +2054,6 @@
     <t>Nichtinvasiver Blutdruck</t>
   </si>
   <si>
-    <t>Elektrokardiograph (EKG) Blei I</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung II</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung III</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung aVR</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung aVL</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Blei aVF</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung V1</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Blei V2</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung V3</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung V4</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung V5</t>
-  </si>
-  <si>
-    <t>Elektrokardiograph (EKG) Ableitung V6</t>
-  </si>
-  <si>
     <t>Electrocardiografía</t>
   </si>
   <si>
@@ -2105,39 +2066,6 @@
     <t>Capnografía del final de la marea</t>
   </si>
   <si>
-    <t>Electrocardiógrafo (ECG) Plomo I</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo II</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo III</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo aVL</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo aVF</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo V1</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo V2</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo V3</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo V4</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo V5</t>
-  </si>
-  <si>
-    <t>Electrocardiógrafo (ECG) Plomo V6</t>
-  </si>
-  <si>
     <t>Eletrocardiograma</t>
   </si>
   <si>
@@ -2279,15 +2207,6 @@
     <t>Неинвазивное кровяное давление</t>
   </si>
   <si>
-    <t>Электрокардиограф View I</t>
-  </si>
-  <si>
-    <t>Электрокардиограф View II</t>
-  </si>
-  <si>
-    <t>Электрокардиограф View III</t>
-  </si>
-  <si>
     <t>Электрокардиограф Посмотреть aVR</t>
   </si>
   <si>
@@ -2313,6 +2232,495 @@
   </si>
   <si>
     <t>Электрокардиограф Посмотреть V6</t>
+  </si>
+  <si>
+    <t>CM:MenuRemoveTracing</t>
+  </si>
+  <si>
+    <t>CM:MenuRemoveNumeric</t>
+  </si>
+  <si>
+    <t>CM:MenuSelectInputSource</t>
+  </si>
+  <si>
+    <t>TRACING:ECG</t>
+  </si>
+  <si>
+    <t>Remove Tracing</t>
+  </si>
+  <si>
+    <t>Remove Numeric</t>
+  </si>
+  <si>
+    <t>Select Input:</t>
+  </si>
+  <si>
+    <t>NUMERIC:PA</t>
+  </si>
+  <si>
+    <t>ECG:WindowTitle</t>
+  </si>
+  <si>
+    <t>ECG:MenuDeviceOptions</t>
+  </si>
+  <si>
+    <t>ECG:MenuPauseDevice</t>
+  </si>
+  <si>
+    <t>ECG:MenuToggleFullscreen</t>
+  </si>
+  <si>
+    <t>ECG:MenuCloseDevice</t>
+  </si>
+  <si>
+    <t>ECG:MenuExitProgram</t>
+  </si>
+  <si>
+    <t>Infirmary Integrated: Electrocardiogram</t>
+  </si>
+  <si>
+    <t>Krankenstation integriert: Elektrokardiograph</t>
+  </si>
+  <si>
+    <t>Enfermería integrada: Electrocardiografía</t>
+  </si>
+  <si>
+    <t>Infirmerie intégrée: Électrocardiographe</t>
+  </si>
+  <si>
+    <t>Infermeria integrata: Elettrocardiografo</t>
+  </si>
+  <si>
+    <t>Infirmary Integrated: Eletrocardiograma</t>
+  </si>
+  <si>
+    <t>Инвалидный комплекс: Электрокардиограф</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_I__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_II__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_III__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_AVR__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_AVL__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_AVF__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_V1__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_V2__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_V3__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_V4__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_V5__SHORT</t>
+  </si>
+  <si>
+    <t>LEAD:ECG_V6__SHORT</t>
+  </si>
+  <si>
+    <t>Lead I</t>
+  </si>
+  <si>
+    <t>Lead II</t>
+  </si>
+  <si>
+    <t>Lead III</t>
+  </si>
+  <si>
+    <t>Lead aVR</t>
+  </si>
+  <si>
+    <t>Lead aVL</t>
+  </si>
+  <si>
+    <t>Lead aVF</t>
+  </si>
+  <si>
+    <t>Lead V1</t>
+  </si>
+  <si>
+    <t>Lead V2</t>
+  </si>
+  <si>
+    <t>Lead V3</t>
+  </si>
+  <si>
+    <t>Lead V4</t>
+  </si>
+  <si>
+    <t>Lead V5</t>
+  </si>
+  <si>
+    <t>Lead V6</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht I</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht aVF</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht V2</t>
+  </si>
+  <si>
+    <t>Aussicht I</t>
+  </si>
+  <si>
+    <t>Aussicht aVF</t>
+  </si>
+  <si>
+    <t>Aussicht V2</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht II</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht III</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht aVR</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht aVL</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht V1</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht V3</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht V4</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht V5</t>
+  </si>
+  <si>
+    <t>Elektrokardiograph (EKG) Aussicht V6</t>
+  </si>
+  <si>
+    <t>Aussicht II</t>
+  </si>
+  <si>
+    <t>Aussicht III</t>
+  </si>
+  <si>
+    <t>Aussicht aVR</t>
+  </si>
+  <si>
+    <t>Aussicht aVL</t>
+  </si>
+  <si>
+    <t>Aussicht V1</t>
+  </si>
+  <si>
+    <t>Aussicht V3</t>
+  </si>
+  <si>
+    <t>Aussicht V4</t>
+  </si>
+  <si>
+    <t>Aussicht V5</t>
+  </si>
+  <si>
+    <t>Aussicht V6</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista I</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista II</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista III</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista aVL</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista aVF</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista V1</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista V2</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista V3</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista V4</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista V5</t>
+  </si>
+  <si>
+    <t>Electrocardiógrafo (ECG) Vista V6</t>
+  </si>
+  <si>
+    <t>Electrocardiograph (ECG) Vista aVR</t>
+  </si>
+  <si>
+    <t>Vista I</t>
+  </si>
+  <si>
+    <t>Vista II</t>
+  </si>
+  <si>
+    <t>Vista III</t>
+  </si>
+  <si>
+    <t>Vista aVL</t>
+  </si>
+  <si>
+    <t>Vista aVF</t>
+  </si>
+  <si>
+    <t>Vista V1</t>
+  </si>
+  <si>
+    <t>Vista V2</t>
+  </si>
+  <si>
+    <t>Vista V3</t>
+  </si>
+  <si>
+    <t>Vista V4</t>
+  </si>
+  <si>
+    <t>Vista V5</t>
+  </si>
+  <si>
+    <t>Vista V6</t>
+  </si>
+  <si>
+    <t>Vista aVR</t>
+  </si>
+  <si>
+    <t>Voir I</t>
+  </si>
+  <si>
+    <t>Voir II</t>
+  </si>
+  <si>
+    <t>Voir III</t>
+  </si>
+  <si>
+    <t>Voir aVR</t>
+  </si>
+  <si>
+    <t>Voir aVL</t>
+  </si>
+  <si>
+    <t>Voir aVF</t>
+  </si>
+  <si>
+    <t>Voir V1</t>
+  </si>
+  <si>
+    <t>Voir V2</t>
+  </si>
+  <si>
+    <t>Voir V3</t>
+  </si>
+  <si>
+    <t>Voir V4</t>
+  </si>
+  <si>
+    <t>Voir V5</t>
+  </si>
+  <si>
+    <t>Voir V6</t>
+  </si>
+  <si>
+    <t>Visualizza I</t>
+  </si>
+  <si>
+    <t>Visualizza  II</t>
+  </si>
+  <si>
+    <t>Visualizza  III</t>
+  </si>
+  <si>
+    <t>Visualizza aVR</t>
+  </si>
+  <si>
+    <t>Visualizza aVL</t>
+  </si>
+  <si>
+    <t>Visualizza aVF</t>
+  </si>
+  <si>
+    <t>Visualizza V1</t>
+  </si>
+  <si>
+    <t>Visualizza V2</t>
+  </si>
+  <si>
+    <t>Visualizza V3</t>
+  </si>
+  <si>
+    <t>Visualizza V4</t>
+  </si>
+  <si>
+    <t>Visualizza V5</t>
+  </si>
+  <si>
+    <t>Visualizza V6</t>
+  </si>
+  <si>
+    <t>Ver I</t>
+  </si>
+  <si>
+    <t>Ver II</t>
+  </si>
+  <si>
+    <t>Ver III</t>
+  </si>
+  <si>
+    <t>Ver aVR</t>
+  </si>
+  <si>
+    <t>Ver aVL</t>
+  </si>
+  <si>
+    <t>Ver aVF</t>
+  </si>
+  <si>
+    <t>Ver V1</t>
+  </si>
+  <si>
+    <t>Ver V2</t>
+  </si>
+  <si>
+    <t>Ver V3</t>
+  </si>
+  <si>
+    <t>Ver V4</t>
+  </si>
+  <si>
+    <t>Ver V5</t>
+  </si>
+  <si>
+    <t>Ver V6</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>aVR</t>
+  </si>
+  <si>
+    <t>aVL</t>
+  </si>
+  <si>
+    <t>aVF</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>Электрокардиограф Посмотреть I</t>
+  </si>
+  <si>
+    <t>Электрокардиограф Посмотреть II</t>
+  </si>
+  <si>
+    <t>Электрокардиограф Посмотреть III</t>
+  </si>
+  <si>
+    <t>Eliminar forma de onda</t>
+  </si>
+  <si>
+    <t>Supprimer la forme d'onde</t>
+  </si>
+  <si>
+    <t>Rimuovi la forma d'onda</t>
+  </si>
+  <si>
+    <t>Remover a forma de onda</t>
+  </si>
+  <si>
+    <t>Saída Infirmary Integrated</t>
+  </si>
+  <si>
+    <t>Удалить форму волны</t>
+  </si>
+  <si>
+    <t>Entfernen Sie die Wellenform</t>
+  </si>
+  <si>
+    <t>Entfernen Sie die Nummern</t>
+  </si>
+  <si>
+    <t>Удалить номера</t>
+  </si>
+  <si>
+    <t>Remova números</t>
+  </si>
+  <si>
+    <t>Rimuovi numeri</t>
+  </si>
+  <si>
+    <t>Supprimer les numéros</t>
+  </si>
+  <si>
+    <t>Eliminar números</t>
+  </si>
+  <si>
+    <t>Seleccionar fuente de entrada</t>
+  </si>
+  <si>
+    <t>Sélectionnez la source d'entrée</t>
+  </si>
+  <si>
+    <t>Seleziona la sorgente di input</t>
+  </si>
+  <si>
+    <t>Selecione a fonte de entrada</t>
+  </si>
+  <si>
+    <t>Выбор источника входного сигнала</t>
+  </si>
+  <si>
+    <t>Wählen Sie die Eingangsquelle</t>
   </si>
 </sst>
 </file>
@@ -2653,11 +3061,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="80.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,7 +3215,7 @@
         <v>452</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>457</v>
@@ -2816,13 +3224,13 @@
         <v>452</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>457</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2833,22 +3241,22 @@
         <v>406</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>458</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2859,22 +3267,22 @@
         <v>407</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>459</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2885,22 +3293,22 @@
         <v>408</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>460</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2911,22 +3319,22 @@
         <v>409</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>461</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2937,19 +3345,19 @@
         <v>410</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>462</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>410</v>
@@ -2963,19 +3371,19 @@
         <v>411</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>411</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>411</v>
@@ -2989,7 +3397,7 @@
         <v>412</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>412</v>
@@ -3004,7 +3412,7 @@
         <v>412</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3015,22 +3423,22 @@
         <v>413</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>413</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>413</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3041,19 +3449,19 @@
         <v>414</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>414</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>414</v>
@@ -3067,22 +3475,22 @@
         <v>415</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>463</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3093,22 +3501,22 @@
         <v>416</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>464</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>464</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3119,22 +3527,22 @@
         <v>417</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>465</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3145,22 +3553,22 @@
         <v>418</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>466</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3171,22 +3579,22 @@
         <v>419</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>467</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3197,22 +3605,22 @@
         <v>420</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>468</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3223,22 +3631,22 @@
         <v>421</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>469</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3249,22 +3657,22 @@
         <v>422</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>470</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3275,22 +3683,22 @@
         <v>423</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>471</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>471</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3301,22 +3709,22 @@
         <v>424</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>472</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3327,22 +3735,22 @@
         <v>425</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>473</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3353,22 +3761,22 @@
         <v>426</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>474</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>426</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3376,25 +3784,25 @@
         <v>450</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>546</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3402,25 +3810,25 @@
         <v>451</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>475</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3431,22 +3839,22 @@
         <v>405</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>476</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3457,22 +3865,22 @@
         <v>455</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>455</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>455</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3483,22 +3891,22 @@
         <v>456</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>456</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>456</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4110,7 +4518,7 @@
         <v>341</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>162</v>
@@ -4122,7 +4530,7 @@
         <v>68</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -4460,7 +4868,7 @@
         <v>263</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4471,22 +4879,22 @@
         <v>394</v>
       </c>
       <c r="C77" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="G77" s="5" t="s">
+      <c r="H77" s="5" t="s">
         <v>645</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4549,22 +4957,22 @@
         <v>403</v>
       </c>
       <c r="C80" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="E80" s="5" t="s">
-        <v>657</v>
-      </c>
       <c r="F80" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="G80" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="H80" s="5" t="s">
         <v>660</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4575,22 +4983,22 @@
         <v>402</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4627,22 +5035,22 @@
         <v>398</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D83" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="E83" s="5" t="s">
-        <v>667</v>
-      </c>
       <c r="F83" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4653,22 +5061,22 @@
         <v>399</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D84" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="F84" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="E84" s="5" t="s">
-        <v>668</v>
-      </c>
-      <c r="F84" s="5" t="s">
+      <c r="G84" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="G84" s="5" t="s">
-        <v>671</v>
-      </c>
       <c r="H84" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4769,842 +5177,1416 @@
         <v>381</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>240</v>
+        <v>884</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>280</v>
       </c>
     </row>
+    <row r="89" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>885</v>
+      </c>
+    </row>
     <row r="90" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>480</v>
+        <v>737</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>477</v>
+        <v>741</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>674</v>
+        <v>887</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>689</v>
+        <v>892</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>719</v>
+        <v>891</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>746</v>
+        <v>890</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>704</v>
+        <v>889</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>749</v>
+        <v>888</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>481</v>
+        <v>738</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>0</v>
+        <v>742</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>340</v>
+        <v>898</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>119</v>
+        <v>893</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>161</v>
+        <v>894</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>119</v>
+        <v>895</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>119</v>
+        <v>896</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>294</v>
-      </c>
-    </row>
+        <v>897</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>483</v>
+        <v>744</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>478</v>
+        <v>750</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>675</v>
+        <v>751</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>690</v>
+        <v>752</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>720</v>
+        <v>753</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>734</v>
+        <v>754</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>705</v>
+        <v>755</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>676</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>691</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>721</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>735</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>706</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
     <row r="100" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>67</v>
+        <v>477</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>339</v>
+        <v>673</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>118</v>
+        <v>676</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>160</v>
+        <v>695</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>212</v>
+        <v>722</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>250</v>
+        <v>680</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>295</v>
+        <v>725</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>214</v>
+        <v>119</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>252</v>
+        <v>119</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>518</v>
+        <v>483</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>71</v>
+        <v>478</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>344</v>
+        <v>674</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>122</v>
+        <v>677</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>165</v>
+        <v>696</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>215</v>
+        <v>710</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>253</v>
+        <v>681</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>299</v>
+        <v>647</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>504</v>
+        <v>484</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>675</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>720</v>
+        <v>697</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>734</v>
+        <v>711</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>705</v>
+        <v>682</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>648</v>
+        <v>726</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>506</v>
+        <v>486</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>489</v>
+        <v>69</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>677</v>
+        <v>342</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>693</v>
+        <v>120</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>733</v>
+        <v>163</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>736</v>
+        <v>213</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>707</v>
+        <v>251</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>751</v>
+        <v>297</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>490</v>
+        <v>70</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>678</v>
+        <v>343</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>694</v>
+        <v>121</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>732</v>
+        <v>164</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>747</v>
+        <v>214</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>711</v>
+        <v>252</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>752</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>508</v>
+        <v>743</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>491</v>
+        <v>71</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>679</v>
+        <v>344</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>695</v>
+        <v>122</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>731</v>
+        <v>165</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>748</v>
+        <v>215</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>710</v>
+        <v>253</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>680</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="G109" s="5" t="s">
-        <v>708</v>
-      </c>
-      <c r="H109" s="5" t="s">
-        <v>754</v>
-      </c>
-    </row>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>510</v>
+        <v>739</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>696</v>
+        <v>676</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>723</v>
+        <v>695</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>712</v>
+        <v>680</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>697</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>724</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>739</v>
-      </c>
-      <c r="G111" s="5" t="s">
-        <v>709</v>
-      </c>
-      <c r="H111" s="5" t="s">
-        <v>756</v>
-      </c>
-    </row>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="112" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>495</v>
+        <v>67</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>683</v>
+        <v>339</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>698</v>
+        <v>118</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>725</v>
+        <v>160</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>740</v>
+        <v>212</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>713</v>
+        <v>250</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>758</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>496</v>
+        <v>70</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>684</v>
+        <v>343</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>699</v>
+        <v>121</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>726</v>
+        <v>164</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>741</v>
+        <v>214</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>714</v>
+        <v>252</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>759</v>
+        <v>298</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>497</v>
+        <v>69</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>685</v>
+        <v>342</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>700</v>
+        <v>120</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>727</v>
+        <v>163</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>742</v>
+        <v>213</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>715</v>
+        <v>251</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>757</v>
+        <v>297</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>498</v>
+        <v>71</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>686</v>
+        <v>344</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>701</v>
+        <v>122</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>728</v>
+        <v>165</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>743</v>
+        <v>215</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>716</v>
+        <v>253</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>760</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>499</v>
+        <v>66</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>687</v>
+        <v>338</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>702</v>
+        <v>117</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>729</v>
+        <v>159</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>744</v>
+        <v>211</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>717</v>
+        <v>249</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>761</v>
+        <v>294</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="C117" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="G117" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="H117" s="5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="G118" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="H118" s="5" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="G119" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="H119" s="5" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>713</v>
+      </c>
+      <c r="G121" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="G122" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="H122" s="5" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="G123" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="H123" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="G124" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="H125" s="5" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="E126" s="5" t="s">
         <v>703</v>
       </c>
-      <c r="E117" s="5" t="s">
+      <c r="F126" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="H126" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="F117" s="5" t="s">
-        <v>745</v>
-      </c>
-      <c r="G117" s="5" t="s">
-        <v>718</v>
-      </c>
-      <c r="H117" s="5" t="s">
+    </row>
+    <row r="127" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="H127" s="5" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="H128" s="5" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>706</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="H129" s="5" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="H130" s="5" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="H131" s="5" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="H133" s="5" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="B135" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>846</v>
+      </c>
+      <c r="G135" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="H135" s="5" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>847</v>
+      </c>
+      <c r="G136" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="H136" s="5" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>823</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="H137" s="5" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>777</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>837</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="G138" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="G139" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="H139" s="5" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>863</v>
+      </c>
+      <c r="H140" s="5" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="G141" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="H141" s="5" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B143" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C143" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D143" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E143" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F119" s="3" t="s">
+      <c r="F143" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G119" s="3" t="s">
+      <c r="G143" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="H119" s="3" t="s">
+      <c r="H143" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B144" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C144" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D120" s="3" t="s">
+      <c r="D144" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E120" s="3" t="s">
+      <c r="E144" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F120" s="3" t="s">
+      <c r="F144" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="G120" s="3" t="s">
+      <c r="G144" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H120" s="3" t="s">
+      <c r="H144" s="3" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C145" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D145" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E145" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F121" s="3" t="s">
+      <c r="F145" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G121" s="3" t="s">
+      <c r="G145" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="H121" s="3" t="s">
+      <c r="H145" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B147" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C147" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D147" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="E147" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F123" s="3" t="s">
+      <c r="F147" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G123" s="3" t="s">
+      <c r="G147" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="H123" s="3" t="s">
+      <c r="H147" s="3" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C148" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D148" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E124" s="3" t="s">
+      <c r="E148" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F124" s="3" t="s">
+      <c r="F148" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="G124" s="3" t="s">
+      <c r="G148" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="H124" s="3" t="s">
+      <c r="H148" s="3" t="s">
         <v>319</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V 0.9.03; IABP Partially Implemented - Patient: Transduced lines need to be zeroed before use   - Added "Zero Transducer" to context menu for MonitorTracing, MonitorNumeric   - Implemented Zero Pressure in DeviceIABP - Waveforms.cs: IABP_ABP_Rhythm, IABP_Balloon_Rhythm implemented   - All ABP strips populate with IABP ABP waveform if IABP is running - DeviceIABP layout: IABPTracings, IABPNumerics, Buttons (top row of control panel only) - DeviceIABP functionality: Start, Pause, Zero Pressure
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="1167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="1177">
   <si>
     <t>Temperature</t>
   </si>
@@ -3515,9 +3515,6 @@
     <t>Auto</t>
   </si>
   <si>
-    <t>Semi-Auto</t>
-  </si>
-  <si>
     <t>Manual</t>
   </si>
   <si>
@@ -3525,6 +3522,39 @@
   </si>
   <si>
     <t>Intra-aortic Balloon Pump</t>
+  </si>
+  <si>
+    <t>IABPBUTTON:Start</t>
+  </si>
+  <si>
+    <t>IABPBUTTON:Pause</t>
+  </si>
+  <si>
+    <t>IABPBUTTON:ZeroPressure</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Zero\nPressure</t>
+  </si>
+  <si>
+    <t>Semi Auto</t>
+  </si>
+  <si>
+    <t>Zero Transducer</t>
+  </si>
+  <si>
+    <t>MENU:MenuZeroTransducer</t>
+  </si>
+  <si>
+    <t>NUMERIC:ZeroTransducer</t>
+  </si>
+  <si>
+    <t>Zero\nTransducer</t>
   </si>
 </sst>
 </file>
@@ -3874,11 +3904,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J168"/>
+  <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B125" sqref="B125"/>
+      <selection pane="topRight" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6707,1528 +6737,1572 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>648</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>651</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>670</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>697</v>
-      </c>
-      <c r="G108" s="5" t="s">
-        <v>953</v>
-      </c>
-      <c r="H108" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="I108" s="5" t="s">
-        <v>700</v>
-      </c>
-      <c r="J108" s="5" t="s">
-        <v>452</v>
+    <row r="107" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>1173</v>
       </c>
     </row>
     <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>0</v>
+        <v>452</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>320</v>
+        <v>648</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>105</v>
+        <v>651</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>146</v>
+        <v>670</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>105</v>
+        <v>697</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>924</v>
+        <v>953</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>105</v>
+        <v>655</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>278</v>
+        <v>700</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>1014</v>
+        <v>452</v>
       </c>
     </row>
     <row r="110" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>196</v>
+        <v>105</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>232</v>
+        <v>105</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="J110" s="5" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="111" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>453</v>
+        <v>52</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>649</v>
+        <v>318</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>652</v>
+        <v>103</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>671</v>
+        <v>144</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>685</v>
+        <v>196</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>954</v>
+        <v>922</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>656</v>
+        <v>232</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>622</v>
+        <v>276</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>1038</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>53</v>
+        <v>453</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>319</v>
+        <v>649</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>104</v>
+        <v>652</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>145</v>
+        <v>671</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>197</v>
+        <v>685</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>923</v>
+        <v>954</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>233</v>
+        <v>656</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>277</v>
+        <v>622</v>
       </c>
       <c r="J112" s="5" t="s">
-        <v>1013</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>454</v>
+        <v>53</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>650</v>
+        <v>319</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>653</v>
+        <v>104</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>672</v>
+        <v>145</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>686</v>
+        <v>197</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>955</v>
+        <v>923</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>657</v>
+        <v>233</v>
       </c>
       <c r="I113" s="5" t="s">
-        <v>701</v>
+        <v>277</v>
       </c>
       <c r="J113" s="5" t="s">
-        <v>1039</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>55</v>
+        <v>454</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>322</v>
+        <v>650</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>106</v>
+        <v>653</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>148</v>
+        <v>672</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>198</v>
+        <v>686</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>925</v>
+        <v>955</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>234</v>
+        <v>657</v>
       </c>
       <c r="I114" s="5" t="s">
-        <v>279</v>
+        <v>701</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>1015</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I115" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
         <v>715</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B117" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C116" s="5" t="s">
+      <c r="C117" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D117" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E116" s="5" t="s">
+      <c r="E117" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F116" s="5" t="s">
+      <c r="F117" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="G116" s="5" t="s">
+      <c r="G117" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="H116" s="5" t="s">
+      <c r="H117" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="I116" s="5" t="s">
+      <c r="I117" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="J116" s="5" t="s">
+      <c r="J117" s="5" t="s">
         <v>1017</v>
       </c>
     </row>
-    <row r="117" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>711</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>648</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>651</v>
-      </c>
-      <c r="E118" s="5" t="s">
-        <v>670</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>697</v>
-      </c>
-      <c r="G118" s="5" t="s">
-        <v>953</v>
-      </c>
-      <c r="H118" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="I118" s="5" t="s">
-        <v>700</v>
-      </c>
-      <c r="J118" s="5" t="s">
-        <v>452</v>
+    <row r="118" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>1176</v>
       </c>
     </row>
     <row r="119" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>475</v>
+        <v>711</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>53</v>
+        <v>452</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>319</v>
+        <v>648</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>104</v>
+        <v>651</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>145</v>
+        <v>670</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>197</v>
+        <v>697</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>923</v>
+        <v>953</v>
       </c>
       <c r="H120" s="5" t="s">
-        <v>233</v>
+        <v>655</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="J120" s="3" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="G121" s="5" t="s">
-        <v>926</v>
-      </c>
-      <c r="H121" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="I121" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J121" s="5" t="s">
-        <v>1016</v>
-      </c>
-    </row>
+        <v>700</v>
+      </c>
+      <c r="J120" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="122" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="J122" s="5" t="s">
-        <v>1015</v>
+        <v>277</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="123" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I123" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J123" s="5" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="124" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G124" s="5" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="I124" s="5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="J124" s="5" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="6" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>1166</v>
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="H125" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="I125" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="J125" s="5" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>453</v>
+        <v>52</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>649</v>
+        <v>318</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>654</v>
+        <v>103</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>671</v>
+        <v>144</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>685</v>
+        <v>196</v>
       </c>
       <c r="G126" s="5" t="s">
-        <v>956</v>
+        <v>922</v>
       </c>
       <c r="H126" s="5" t="s">
-        <v>656</v>
+        <v>232</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="J126" s="3" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>748</v>
-      </c>
-      <c r="D127" s="5" t="s">
-        <v>772</v>
-      </c>
-      <c r="E127" s="5" t="s">
-        <v>684</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>687</v>
-      </c>
-      <c r="G127" s="5" t="s">
-        <v>957</v>
-      </c>
-      <c r="H127" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="I127" s="5" t="s">
-        <v>844</v>
-      </c>
-      <c r="J127" s="5" t="s">
-        <v>1083</v>
+        <v>276</v>
+      </c>
+      <c r="J126" s="5" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>1165</v>
       </c>
     </row>
     <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>754</v>
+        <v>649</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>773</v>
+        <v>654</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>683</v>
+        <v>671</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="H128" s="5" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="I128" s="5" t="s">
-        <v>845</v>
-      </c>
-      <c r="J128" s="5" t="s">
-        <v>1084</v>
+        <v>622</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>1057</v>
       </c>
     </row>
     <row r="129" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>755</v>
+        <v>748</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>699</v>
+        <v>687</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="H129" s="5" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="I129" s="5" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="J129" s="5" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="130" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>673</v>
+        <v>683</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="H130" s="5" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="I130" s="5" t="s">
-        <v>702</v>
+        <v>845</v>
       </c>
       <c r="J130" s="5" t="s">
-        <v>1074</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>689</v>
+        <v>699</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>1094</v>
+        <v>959</v>
       </c>
       <c r="H131" s="5" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I131" s="5" t="s">
-        <v>703</v>
+        <v>846</v>
       </c>
       <c r="J131" s="5" t="s">
-        <v>1075</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>1095</v>
+        <v>960</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I132" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="J132" s="5" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="133" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>961</v>
+        <v>1094</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I133" s="5" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="J133" s="5" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="134" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G134" s="5" t="s">
-        <v>962</v>
+        <v>1095</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="I134" s="5" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="J134" s="5" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="135" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I135" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="J135" s="5" t="s">
-        <v>1077</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="136" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G136" s="5" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I136" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="J136" s="5" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="137" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="I137" s="5" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="J137" s="5" t="s">
-        <v>1082</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G138" s="5" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="I138" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="J138" s="5" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>724</v>
+        <v>490</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>736</v>
+        <v>473</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>751</v>
+        <v>761</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>796</v>
+        <v>680</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>808</v>
+        <v>695</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="H139" s="5" t="s">
-        <v>820</v>
+        <v>668</v>
       </c>
       <c r="I139" s="5" t="s">
-        <v>832</v>
+        <v>709</v>
       </c>
       <c r="J139" s="5" t="s">
-        <v>1062</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>725</v>
+        <v>491</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>737</v>
+        <v>474</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>797</v>
+        <v>681</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>809</v>
+        <v>696</v>
       </c>
       <c r="G140" s="5" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="H140" s="5" t="s">
-        <v>821</v>
+        <v>669</v>
       </c>
       <c r="I140" s="5" t="s">
-        <v>833</v>
+        <v>710</v>
       </c>
       <c r="J140" s="5" t="s">
-        <v>1063</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="H141" s="5" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="I141" s="5" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="J141" s="5" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="G142" s="5" t="s">
-        <v>1097</v>
+        <v>968</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="I142" s="5" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="J142" s="5" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="143" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F143" s="5" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>1096</v>
+        <v>969</v>
       </c>
       <c r="H143" s="5" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="J143" s="5" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="144" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>752</v>
+        <v>765</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>788</v>
+        <v>795</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F144" s="5" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G144" s="5" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="H144" s="5" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I144" s="5" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="J144" s="5" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="145" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F145" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>970</v>
+        <v>1096</v>
       </c>
       <c r="H145" s="5" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="I145" s="5" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="J145" s="5" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="146" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G146" s="5" t="s">
-        <v>971</v>
+        <v>1098</v>
       </c>
       <c r="H146" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I146" s="5" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="J146" s="5" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="147" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F147" s="5" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="H147" s="5" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="I147" s="5" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="J147" s="5" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="148" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>769</v>
+        <v>753</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I148" s="5" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="J148" s="5" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="149" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F149" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="I149" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="J149" s="5" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="150" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="G150" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="H150" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="I150" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="J150" s="5" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="F151" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="G151" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="H151" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="I151" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="J151" s="5" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B152" s="5" t="s">
         <v>747</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C152" s="5" t="s">
         <v>771</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D152" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="E150" s="5" t="s">
+      <c r="E152" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="F150" s="5" t="s">
+      <c r="F152" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="G150" s="5" t="s">
+      <c r="G152" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="H150" s="5" t="s">
+      <c r="H152" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="I150" s="5" t="s">
+      <c r="I152" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="J150" s="5" t="s">
+      <c r="J152" s="5" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="151" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="6" t="s">
-        <v>1121</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="6" t="s">
-        <v>1122</v>
-      </c>
-      <c r="B153" s="6" t="s">
-        <v>1126</v>
-      </c>
-    </row>
+    <row r="153" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="154" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="155" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="6" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>1127</v>
+      </c>
+    </row>
     <row r="157" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
-        <v>1155</v>
+        <v>1124</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="6" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B158" s="6" t="s">
-        <v>1158</v>
-      </c>
-    </row>
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="159" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="160" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="161" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="6" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
         <v>1161</v>
       </c>
-      <c r="B161" s="6" t="s">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+      <c r="B163" s="6" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B172" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C172" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="D163" s="3" t="s">
+      <c r="D172" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E163" s="3" t="s">
+      <c r="E172" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F163" s="3" t="s">
+      <c r="F172" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G163" s="3" t="s">
+      <c r="G172" s="3" t="s">
         <v>911</v>
       </c>
-      <c r="H163" s="3" t="s">
+      <c r="H172" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="I163" s="3" t="s">
+      <c r="I172" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="J163" s="3" t="s">
+      <c r="J172" s="3" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B173" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C164" s="3" t="s">
+      <c r="C173" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D164" s="3" t="s">
+      <c r="D173" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E164" s="3" t="s">
+      <c r="E173" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F164" s="3" t="s">
+      <c r="F173" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="G164" s="3" t="s">
+      <c r="G173" s="3" t="s">
         <v>976</v>
       </c>
-      <c r="H164" s="3" t="s">
+      <c r="H173" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="I164" s="3" t="s">
+      <c r="I173" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="J164" s="3" t="s">
+      <c r="J173" s="3" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B174" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C165" s="3" t="s">
+      <c r="C174" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D165" s="3" t="s">
+      <c r="D174" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E165" s="3" t="s">
+      <c r="E174" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F165" s="3" t="s">
+      <c r="F174" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G165" s="3" t="s">
+      <c r="G174" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="H165" s="3" t="s">
+      <c r="H174" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="I165" s="3" t="s">
+      <c r="I174" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="J165" s="3" t="s">
+      <c r="J174" s="3" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B176" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C176" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="D167" s="3" t="s">
+      <c r="D176" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E167" s="3" t="s">
+      <c r="E176" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F167" s="3" t="s">
+      <c r="F176" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G167" s="3" t="s">
+      <c r="G176" s="3" t="s">
         <v>978</v>
       </c>
-      <c r="H167" s="3" t="s">
+      <c r="H176" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I167" s="3" t="s">
+      <c r="I176" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="J167" s="3" t="s">
+      <c r="J176" s="3" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B177" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C168" s="3" t="s">
+      <c r="C177" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D177" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E168" s="3" t="s">
+      <c r="E177" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F168" s="3" t="s">
+      <c r="F177" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G168" s="3" t="s">
+      <c r="G177" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="H168" s="3" t="s">
+      <c r="H177" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="I168" s="3" t="s">
+      <c r="I177" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="J168" s="3" t="s">
+      <c r="J177" s="3" t="s">
         <v>1043</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- V 0.91.06; IABP Augmentation & UI improvments 	- DeviceIABP 		- Augmentation numeric reability improved, updates smoother on setting adjustments 		- Augmentation alarm functional (flashes red/blue if below alarm limit) 		- Left-hand panel readability improvements (font size, color)
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E44740A-8D60-4FC6-BBA5-EA0C197EEB16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710DEE14-9A27-4EEC-890A-BD4E2C8AC3AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="1340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="1338">
   <si>
     <t>Temperature</t>
   </si>
@@ -3570,12 +3570,6 @@
     <t>Augmentation Pressure</t>
   </si>
   <si>
-    <t>IABP:HeliumTank</t>
-  </si>
-  <si>
-    <t>Helium Tank</t>
-  </si>
-  <si>
     <t>IABP:Paused</t>
   </si>
   <si>
@@ -3897,30 +3891,6 @@
     <t>Воздушный шар пуст</t>
   </si>
   <si>
-    <t>Гелиевый резервуар</t>
-  </si>
-  <si>
-    <t>Heli ya tani</t>
-  </si>
-  <si>
-    <t>Serbatoio di elio</t>
-  </si>
-  <si>
-    <t>헬륨 탱크</t>
-  </si>
-  <si>
-    <t>Tanque de hélio</t>
-  </si>
-  <si>
-    <t>Tanque de helio</t>
-  </si>
-  <si>
-    <t>Réservoir d'hélium</t>
-  </si>
-  <si>
-    <t>Heliumtank</t>
-  </si>
-  <si>
     <t>Infirmary Integrated: Bomba de balão intra-aórtico</t>
   </si>
   <si>
@@ -4045,6 +4015,30 @@
   </si>
   <si>
     <t>Frequency</t>
+  </si>
+  <si>
+    <t>IABP:Augmentation</t>
+  </si>
+  <si>
+    <t>IABP:Alarm</t>
+  </si>
+  <si>
+    <t>IABP:Pressure</t>
+  </si>
+  <si>
+    <t>Augmentation</t>
+  </si>
+  <si>
+    <t>Alarm</t>
+  </si>
+  <si>
+    <t>NUMERIC:IABP_AP</t>
+  </si>
+  <si>
+    <t>Helium</t>
+  </si>
+  <si>
+    <t>IABP:Helium</t>
   </si>
 </sst>
 </file>
@@ -4392,11 +4386,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J186"/>
+  <dimension ref="A1:J190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B103" sqref="B1:B1048576"/>
+      <selection pane="topRight" activeCell="B94" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4573,28 +4567,28 @@
         <v>1177</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -4605,28 +4599,28 @@
         <v>1178</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>1209</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>1210</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>1211</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>1212</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -6837,2651 +6831,2683 @@
         <v>1154</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>1304</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>1303</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>1302</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>1314</v>
-      </c>
       <c r="G94" s="2" t="s">
-        <v>1301</v>
+        <v>1291</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>1298</v>
+        <v>1288</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>1299</v>
+        <v>1289</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>1320</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>1312</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>1313</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>1315</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>1316</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>1317</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>1318</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>1319</v>
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>1333</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>1180</v>
+        <v>1174</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>1321</v>
+        <v>1310</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>1322</v>
+        <v>1302</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>1323</v>
+        <v>1303</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>1324</v>
+        <v>1305</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>1325</v>
+        <v>1306</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>1326</v>
+        <v>1307</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>1327</v>
+        <v>1308</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>1328</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>1297</v>
+        <v>1311</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>1295</v>
+        <v>1312</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>1296</v>
+        <v>1313</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>1292</v>
+        <v>1314</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>1293</v>
+        <v>1315</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>1294</v>
+        <v>1316</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>1290</v>
+        <v>1317</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>1183</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>1203</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>1209</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>1210</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>1211</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>1212</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>1208</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>1206</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>1184</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>1186</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>1202</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>1215</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>1207</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>1205</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>1278</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>1274</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>1277</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>1285</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>1284</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>1283</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>1286</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>1287</v>
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>1336</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>1331</v>
+        <v>1181</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>1330</v>
+        <v>1183</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>1279</v>
+        <v>1201</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>1275</v>
+        <v>1207</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>1276</v>
+        <v>1208</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>1280</v>
+        <v>1209</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>1281</v>
+        <v>1210</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>1282</v>
+        <v>1206</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>1289</v>
+        <v>1204</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>1288</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>1155</v>
+        <v>1182</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>1157</v>
+        <v>1184</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>648</v>
+        <v>1200</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>651</v>
+        <v>1199</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>670</v>
+        <v>1213</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>697</v>
+        <v>1212</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>953</v>
+        <v>1211</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>655</v>
+        <v>1205</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>700</v>
+        <v>1203</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>452</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>1156</v>
+        <v>1186</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>1158</v>
+        <v>1185</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>322</v>
+        <v>1276</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>106</v>
+        <v>1272</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>1329</v>
+        <v>1275</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>198</v>
+        <v>1283</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>925</v>
+        <v>1282</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>234</v>
+        <v>1281</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>279</v>
+        <v>1284</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>1015</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>1159</v>
+        <v>1321</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>1161</v>
+        <v>1320</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>1224</v>
+        <v>1277</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>1225</v>
+        <v>1273</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>1216</v>
+        <v>1274</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>1220</v>
+        <v>1278</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>1217</v>
+        <v>1279</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>1225</v>
+        <v>1280</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>1228</v>
+        <v>1287</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>1229</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>1169</v>
+        <v>1157</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>1223</v>
+        <v>648</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>1222</v>
+        <v>651</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>1219</v>
+        <v>670</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>1221</v>
+        <v>697</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>1218</v>
+        <v>953</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>1226</v>
+        <v>655</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>1227</v>
+        <v>700</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>1230</v>
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>1164</v>
+        <v>1156</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>1167</v>
+        <v>1158</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>1244</v>
+        <v>322</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>1245</v>
+        <v>106</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>1240</v>
+        <v>1319</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>1239</v>
+        <v>198</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>1238</v>
+        <v>925</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>1232</v>
+        <v>234</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>1233</v>
+        <v>279</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>1231</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>1165</v>
+        <v>1159</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>1168</v>
+        <v>1161</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>1243</v>
+        <v>1222</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>1246</v>
+        <v>1223</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>1241</v>
+        <v>1214</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>1242</v>
-      </c>
-      <c r="G107" s="4" t="s">
-        <v>1237</v>
+        <v>1218</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>1215</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>1235</v>
+        <v>1223</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>1234</v>
+        <v>1226</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>1236</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>1189</v>
+        <v>1169</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>1192</v>
+        <v>1221</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>1193</v>
+        <v>1220</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>1194</v>
+        <v>1217</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>1195</v>
+        <v>1219</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>1196</v>
+        <v>1216</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>1197</v>
+        <v>1224</v>
       </c>
       <c r="I108" s="2" t="s">
-        <v>1198</v>
+        <v>1225</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>1336</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>1339</v>
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>1237</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>1234</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>1190</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>1191</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>1306</v>
-      </c>
       <c r="E111" s="2" t="s">
-        <v>1305</v>
+        <v>1192</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>1308</v>
+        <v>1193</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>1284</v>
+        <v>1194</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>1309</v>
+        <v>1195</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>1310</v>
+        <v>1196</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>1311</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="112" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>1334</v>
+        <v>1327</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="113" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>1335</v>
+        <v>1326</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1333</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>939</v>
-      </c>
-      <c r="H115" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I115" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="J115" s="2" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>940</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="J116" s="2" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>941</v>
-      </c>
-      <c r="H117" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="I117" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>1027</v>
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>1323</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>377</v>
+        <v>75</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>628</v>
+        <v>335</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>627</v>
+        <v>174</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>626</v>
+        <v>160</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>625</v>
+        <v>208</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>624</v>
+        <v>247</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>623</v>
+        <v>291</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>647</v>
+        <v>629</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>642</v>
+        <v>626</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>644</v>
+        <v>625</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>645</v>
+        <v>624</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>79</v>
+        <v>375</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>339</v>
+        <v>647</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>176</v>
+        <v>640</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>164</v>
+        <v>641</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>212</v>
+        <v>639</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>251</v>
+        <v>638</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>295</v>
+        <v>637</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>80</v>
+        <v>376</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>340</v>
+        <v>646</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>177</v>
+        <v>643</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>165</v>
+        <v>642</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>213</v>
+        <v>644</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>252</v>
+        <v>645</v>
       </c>
       <c r="I124" s="2" t="s">
-        <v>296</v>
+        <v>636</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>359</v>
+        <v>119</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>360</v>
+        <v>163</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>361</v>
+        <v>211</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>907</v>
+        <v>946</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>851</v>
+        <v>250</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
       <c r="J125" s="2" t="s">
-        <v>999</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>712</v>
+        <v>79</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>853</v>
+        <v>339</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>847</v>
+        <v>176</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>848</v>
+        <v>164</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>849</v>
+        <v>212</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>850</v>
+        <v>251</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>852</v>
+        <v>295</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>713</v>
+        <v>80</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>854</v>
+        <v>340</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>859</v>
+        <v>177</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>858</v>
+        <v>165</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>857</v>
+        <v>213</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>856</v>
+        <v>252</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>855</v>
+        <v>296</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>714</v>
+        <v>47</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>865</v>
+        <v>358</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>860</v>
+        <v>359</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>861</v>
+        <v>360</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>862</v>
+        <v>361</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>951</v>
+        <v>907</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>863</v>
+        <v>851</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>864</v>
+        <v>263</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>1037</v>
+        <v>999</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>1171</v>
+        <v>1150</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>1170</v>
+        <v>712</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>1192</v>
+        <v>853</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>1193</v>
+        <v>847</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>1194</v>
+        <v>848</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>1195</v>
+        <v>849</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>1196</v>
+        <v>949</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>1197</v>
+        <v>850</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>1198</v>
+        <v>852</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>1199</v>
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="J130" s="2" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>455</v>
+        <v>1152</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>452</v>
+        <v>714</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>648</v>
+        <v>865</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>651</v>
+        <v>860</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>670</v>
+        <v>861</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>697</v>
+        <v>862</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>655</v>
+        <v>863</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>700</v>
+        <v>864</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>452</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>456</v>
+        <v>1171</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>0</v>
+        <v>1170</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>320</v>
+        <v>1190</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>105</v>
+        <v>1191</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>146</v>
+        <v>1192</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>105</v>
+        <v>1193</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>924</v>
+        <v>1194</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>105</v>
+        <v>1195</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>278</v>
+        <v>1196</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G133" s="2" t="s">
-        <v>922</v>
-      </c>
-      <c r="H133" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="I133" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="J133" s="2" t="s">
-        <v>1012</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>685</v>
+        <v>697</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>622</v>
+        <v>700</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>1038</v>
+        <v>452</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>197</v>
+        <v>105</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>233</v>
+        <v>105</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>454</v>
+        <v>52</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>650</v>
+        <v>318</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>653</v>
+        <v>103</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>672</v>
+        <v>144</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>686</v>
+        <v>196</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>955</v>
+        <v>922</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>657</v>
+        <v>232</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>701</v>
+        <v>276</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>1039</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>55</v>
+        <v>453</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>322</v>
+        <v>649</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>106</v>
+        <v>652</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>148</v>
+        <v>671</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>198</v>
+        <v>685</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>925</v>
+        <v>954</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>234</v>
+        <v>656</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>279</v>
+        <v>622</v>
       </c>
       <c r="J137" s="2" t="s">
-        <v>1015</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J138" s="2" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>715</v>
+        <v>460</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>57</v>
+        <v>454</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>324</v>
+        <v>650</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>108</v>
+        <v>653</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>150</v>
+        <v>672</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>200</v>
+        <v>686</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>927</v>
+        <v>955</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>236</v>
+        <v>657</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>281</v>
+        <v>701</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>1017</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>1172</v>
+        <v>461</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>1170</v>
+        <v>55</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>1192</v>
+        <v>322</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>1193</v>
+        <v>106</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>1194</v>
+        <v>148</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>1195</v>
+        <v>198</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>1196</v>
+        <v>925</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>1197</v>
+        <v>234</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>1198</v>
+        <v>279</v>
       </c>
       <c r="J140" s="2" t="s">
-        <v>1199</v>
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I141" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="J141" s="2" t="s">
+        <v>1016</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>452</v>
+        <v>57</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>648</v>
+        <v>324</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>651</v>
+        <v>108</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>670</v>
+        <v>150</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>697</v>
+        <v>200</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>953</v>
+        <v>927</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>655</v>
+        <v>236</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>700</v>
+        <v>281</v>
       </c>
       <c r="J142" s="2" t="s">
-        <v>452</v>
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>1315</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="I143" s="2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="J143" s="2" t="s">
+        <v>1318</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>475</v>
+        <v>1172</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>53</v>
+        <v>1170</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>319</v>
+        <v>1190</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>104</v>
+        <v>1191</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>145</v>
+        <v>1192</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>197</v>
+        <v>1193</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>923</v>
+        <v>1194</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>233</v>
+        <v>1195</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>277</v>
+        <v>1196</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F145" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G145" s="2" t="s">
-        <v>926</v>
-      </c>
-      <c r="H145" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I145" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="J145" s="2" t="s">
-        <v>1016</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>477</v>
+        <v>711</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>55</v>
+        <v>452</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>322</v>
+        <v>648</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>106</v>
+        <v>651</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>148</v>
+        <v>670</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>198</v>
+        <v>697</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>925</v>
+        <v>953</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>234</v>
+        <v>655</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>279</v>
+        <v>700</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G147" s="2" t="s">
-        <v>927</v>
-      </c>
-      <c r="H147" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I147" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="J147" s="2" t="s">
-        <v>1017</v>
+        <v>452</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>1012</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>1162</v>
+        <v>476</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>1163</v>
+        <v>56</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>917</v>
+        <v>926</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>1007</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>453</v>
+        <v>55</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>649</v>
+        <v>322</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>654</v>
+        <v>106</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>671</v>
+        <v>148</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>685</v>
+        <v>198</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>956</v>
+        <v>925</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>656</v>
+        <v>234</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>622</v>
+        <v>279</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>1057</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>463</v>
+        <v>57</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>748</v>
+        <v>324</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>772</v>
+        <v>108</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>684</v>
+        <v>150</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>687</v>
+        <v>200</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>957</v>
+        <v>927</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>658</v>
+        <v>236</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>844</v>
+        <v>281</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>1083</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>464</v>
+        <v>52</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>754</v>
+        <v>318</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>773</v>
+        <v>103</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>683</v>
+        <v>144</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>698</v>
+        <v>196</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>958</v>
+        <v>922</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>662</v>
+        <v>232</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>845</v>
+        <v>276</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>1084</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>482</v>
+        <v>1162</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>465</v>
+        <v>1163</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>755</v>
+        <v>313</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>774</v>
+        <v>98</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>682</v>
+        <v>139</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>699</v>
+        <v>191</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>959</v>
+        <v>917</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>661</v>
+        <v>228</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>846</v>
+        <v>271</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>1085</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>756</v>
+        <v>649</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>783</v>
+        <v>654</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>702</v>
+        <v>622</v>
       </c>
       <c r="J154" s="2" t="s">
-        <v>1074</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>757</v>
+        <v>748</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>1094</v>
+        <v>957</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>703</v>
+        <v>844</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>1075</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>690</v>
+        <v>698</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>1095</v>
+        <v>958</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>704</v>
+        <v>845</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>1076</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>691</v>
+        <v>699</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>706</v>
+        <v>846</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>1080</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="I158" s="2" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="J158" s="2" t="s">
-        <v>1081</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>963</v>
+        <v>1094</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>760</v>
+        <v>749</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>964</v>
+        <v>1095</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>762</v>
+        <v>750</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>724</v>
+        <v>488</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>736</v>
+        <v>471</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>796</v>
+        <v>678</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>808</v>
+        <v>693</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>820</v>
+        <v>666</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>832</v>
+        <v>705</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>1062</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>725</v>
+        <v>489</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>737</v>
+        <v>472</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>797</v>
+        <v>679</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>809</v>
+        <v>694</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>821</v>
+        <v>667</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>833</v>
+        <v>708</v>
       </c>
       <c r="J164" s="2" t="s">
-        <v>1063</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>726</v>
+        <v>490</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>738</v>
+        <v>473</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>798</v>
+        <v>680</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>810</v>
+        <v>695</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>822</v>
+        <v>668</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>834</v>
+        <v>709</v>
       </c>
       <c r="J165" s="2" t="s">
-        <v>1064</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>727</v>
+        <v>491</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>739</v>
+        <v>474</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>799</v>
+        <v>681</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>811</v>
+        <v>696</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>1097</v>
+        <v>966</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>823</v>
+        <v>669</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>835</v>
+        <v>710</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>1065</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>766</v>
+        <v>751</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>1096</v>
+        <v>967</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>752</v>
+        <v>763</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>1098</v>
+        <v>968</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="J169" s="2" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>753</v>
+        <v>765</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>971</v>
+        <v>1097</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>972</v>
+        <v>1096</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>769</v>
+        <v>752</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>973</v>
+        <v>1098</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="I173" s="2" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>771</v>
+        <v>753</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="J174" s="2" t="s">
-        <v>1073</v>
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="G175" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="I175" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>1070</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>1121</v>
+        <v>733</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>1125</v>
+        <v>745</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>1248</v>
+        <v>769</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>1247</v>
+        <v>792</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>1125</v>
+        <v>805</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>1265</v>
+        <v>817</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>1264</v>
+        <v>973</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>1247</v>
+        <v>829</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>1266</v>
+        <v>841</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>1267</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>1122</v>
+        <v>734</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>1126</v>
+        <v>746</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>1250</v>
+        <v>770</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>1251</v>
+        <v>793</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>1249</v>
+        <v>806</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>1261</v>
+        <v>818</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>1262</v>
+        <v>974</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>1263</v>
+        <v>830</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>1273</v>
+        <v>842</v>
       </c>
       <c r="J177" s="2" t="s">
-        <v>1272</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>1123</v>
+        <v>735</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>1127</v>
+        <v>747</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>1253</v>
+        <v>771</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>1252</v>
+        <v>794</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>1254</v>
+        <v>807</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>1259</v>
+        <v>819</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>1260</v>
+        <v>975</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>1252</v>
+        <v>831</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>1270</v>
+        <v>843</v>
       </c>
       <c r="J178" s="2" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
-        <v>1124</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>1257</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>1255</v>
-      </c>
-      <c r="F179" s="2" t="s">
-        <v>1256</v>
-      </c>
-      <c r="G179" s="2" t="s">
-        <v>1258</v>
-      </c>
-      <c r="H179" s="2" t="s">
-        <v>1256</v>
-      </c>
-      <c r="I179" s="2" t="s">
-        <v>1269</v>
-      </c>
-      <c r="J179" s="2" t="s">
-        <v>1268</v>
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>1262</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="I180" s="2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="J180" s="2" t="s">
+        <v>1265</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>40</v>
+        <v>1122</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>82</v>
+        <v>1126</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>309</v>
+        <v>1248</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>120</v>
+        <v>1249</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>133</v>
+        <v>1247</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>185</v>
+        <v>1259</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>911</v>
+        <v>1260</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>226</v>
+        <v>1261</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>265</v>
+        <v>1271</v>
       </c>
       <c r="J181" s="2" t="s">
-        <v>1003</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>38</v>
+        <v>1123</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>84</v>
+        <v>1127</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>84</v>
+        <v>1251</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>122</v>
+        <v>1250</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>84</v>
+        <v>1252</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>215</v>
+        <v>1257</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>976</v>
+        <v>1258</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>253</v>
+        <v>1250</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>298</v>
+        <v>1268</v>
       </c>
       <c r="J182" s="2" t="s">
-        <v>1040</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>39</v>
+        <v>1124</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>85</v>
+        <v>1128</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>342</v>
+        <v>1255</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>123</v>
+        <v>1254</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>167</v>
+        <v>1253</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>216</v>
+        <v>1254</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>977</v>
+        <v>1256</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>254</v>
+        <v>1254</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>299</v>
+        <v>1267</v>
       </c>
       <c r="J183" s="2" t="s">
-        <v>1041</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>978</v>
+        <v>911</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="J185" s="2" t="s">
-        <v>1042</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G186" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="H186" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I186" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J186" s="2" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G187" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="H187" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="I187" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J187" s="2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="H189" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I189" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J189" s="2" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B190" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C190" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D186" s="2" t="s">
+      <c r="D190" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E186" s="2" t="s">
+      <c r="E190" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F186" s="2" t="s">
+      <c r="F190" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G186" s="2" t="s">
+      <c r="G190" s="2" t="s">
         <v>979</v>
       </c>
-      <c r="H186" s="2" t="s">
+      <c r="H190" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="I186" s="2" t="s">
+      <c r="I190" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J186" s="2" t="s">
+      <c r="J190" s="2" t="s">
         <v>1043</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- V 0.91.07; Defibrillator layout and functionality, IABP variable refactoring and logic tweaking 	- DeviceIABP 		- Variables refactored (device settings stored in DeviceIABP, patient results stored in App.Patient) 			- Tracings updated/modified based on activity from DeviceIABP 		- Trigger logic tweaked for realism with different cardiac rhythms (only ECG trigger works for PEA, etc.) 	- DeviceDefib 		- Layout for numerics, tracings, and buttons completed 		- Implemented functionality for all toggling buttons (mode changes and energy selections) 			- Placeholder ExceptionNotImplemented for remaining buttons 		- Implemented defibrillator numeric for device status (mode, energy selected)
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710DEE14-9A27-4EEC-890A-BD4E2C8AC3AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE70273-9654-4CC0-941C-E69EA0FAA313}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="1338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="1384">
   <si>
     <t>Temperature</t>
   </si>
@@ -4039,6 +4039,144 @@
   </si>
   <si>
     <t>IABP:Helium</t>
+  </si>
+  <si>
+    <t>DEFIB:On</t>
+  </si>
+  <si>
+    <t>DEFIB:WindowTitle</t>
+  </si>
+  <si>
+    <t>Infirmary Integrated: Defibrillator</t>
+  </si>
+  <si>
+    <t>DEFIB:Charge</t>
+  </si>
+  <si>
+    <t>DEFIB:Shock</t>
+  </si>
+  <si>
+    <t>DEFIB:Analyze</t>
+  </si>
+  <si>
+    <t>DEFIB:Sync</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Shock</t>
+  </si>
+  <si>
+    <t>Analyze</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>AED Mode</t>
+  </si>
+  <si>
+    <t>DEFIB:AutomaticMode</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DEFIB:EnergyAmount</t>
+  </si>
+  <si>
+    <t>Energy Amount</t>
+  </si>
+  <si>
+    <t>DEFIB:Increase</t>
+  </si>
+  <si>
+    <t>DEFIB:Decrease</t>
+  </si>
+  <si>
+    <t>DEFIB:Pacer</t>
+  </si>
+  <si>
+    <t>DEFIB:Rate</t>
+  </si>
+  <si>
+    <t>DEFIB:Pause</t>
+  </si>
+  <si>
+    <t>Pacer</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Defibrillator Settings</t>
+  </si>
+  <si>
+    <t>NUMERIC:DEFIB</t>
+  </si>
+  <si>
+    <t>DEFIB:Defibrillation</t>
+  </si>
+  <si>
+    <t>DEFIB:Synchronized</t>
+  </si>
+  <si>
+    <t>Defibrillation</t>
+  </si>
+  <si>
+    <t>Synchronized</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>DEFIB:Pacing</t>
+  </si>
+  <si>
+    <t>Pacing</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>DEFIB:ShockAdvised</t>
+  </si>
+  <si>
+    <t>DEFIB:NoShockAdvised</t>
+  </si>
+  <si>
+    <t>DEFIB:StandClear</t>
+  </si>
+  <si>
+    <t>DEFIB:Analyzing</t>
+  </si>
+  <si>
+    <t>Stand Clear</t>
+  </si>
+  <si>
+    <t>Shock Advised</t>
+  </si>
+  <si>
+    <t>Analyzing</t>
+  </si>
+  <si>
+    <t>No Shock Advised</t>
+  </si>
+  <si>
+    <t>DEFIB:ContinueCPR</t>
+  </si>
+  <si>
+    <t>Continue CPR</t>
+  </si>
+  <si>
+    <t>DEFIB:Joules</t>
+  </si>
+  <si>
+    <t>DEFIB:Milliamps</t>
   </si>
 </sst>
 </file>
@@ -4082,12 +4220,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -4096,16 +4249,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4386,11 +4539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J190"/>
+  <dimension ref="A1:J216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B94" sqref="B1:B1048576"/>
+      <selection pane="topRight" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6857,2657 +7010,2849 @@
     </row>
     <row r="95" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>1330</v>
+        <v>1339</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1333</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>1302</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>1303</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>1305</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>1306</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>1307</v>
-      </c>
-      <c r="I96" s="2" t="s">
-        <v>1308</v>
-      </c>
-      <c r="J96" s="2" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>1179</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>1311</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>1312</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>1313</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>1314</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>1315</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>1316</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>1317</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>1331</v>
+        <v>1355</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>1332</v>
+        <v>1356</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>1337</v>
+        <v>1353</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>1181</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>1183</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>1201</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>1207</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>1208</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>1209</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>1210</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>1206</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>1204</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>1182</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>1199</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>1213</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>1212</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>1211</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>1203</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>1276</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>1272</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>1275</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>1283</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>1282</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>1281</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>1284</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>1285</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>1320</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>1277</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>1273</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>1274</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>1278</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>1279</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>1280</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>1287</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>1155</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>1157</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>953</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="I105" s="2" t="s">
-        <v>700</v>
-      </c>
-      <c r="J105" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>1158</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>1319</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>1218</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>1215</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>1223</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>1226</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>1220</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>1217</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>1219</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>1216</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>1224</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>1225</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>1242</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>1243</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>1238</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>1237</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>1236</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>1230</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>1231</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B110" s="2" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>1168</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>1241</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>1244</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>1240</v>
-      </c>
-      <c r="G110" s="4" t="s">
-        <v>1235</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>1233</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>1232</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>1192</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>1193</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>1194</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>1195</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>1196</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>1327</v>
+        <v>1382</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1328</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="113" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>1326</v>
+        <v>1383</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>1297</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>1296</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>1295</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>1298</v>
-      </c>
-      <c r="G114" s="2" t="s">
-        <v>1282</v>
-      </c>
-      <c r="H114" s="2" t="s">
-        <v>1299</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>1300</v>
-      </c>
-      <c r="J114" s="2" t="s">
-        <v>1301</v>
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>1376</v>
       </c>
     </row>
     <row r="115" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>1324</v>
+        <v>1375</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1322</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="116" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>1325</v>
+        <v>1372</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>939</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="J118" s="2" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>940</v>
-      </c>
-      <c r="H119" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="J119" s="2" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>941</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="I120" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>1027</v>
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>1333</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>1142</v>
+        <v>1173</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>377</v>
+        <v>1174</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>628</v>
+        <v>1310</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>627</v>
+        <v>1302</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>626</v>
+        <v>1303</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>625</v>
+        <v>1305</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>942</v>
+        <v>1306</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>624</v>
+        <v>1307</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>623</v>
+        <v>1308</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>1028</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>1143</v>
+        <v>1179</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>77</v>
+        <v>1180</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>337</v>
+        <v>1311</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>118</v>
+        <v>1312</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>162</v>
+        <v>1313</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>210</v>
+        <v>1314</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>943</v>
+        <v>1315</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>249</v>
+        <v>1316</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>293</v>
+        <v>1317</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>1144</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="G123" s="2" t="s">
-        <v>944</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="I123" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="J123" s="2" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="G124" s="2" t="s">
-        <v>945</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="I124" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="J124" s="2" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>1146</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>946</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I125" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>1032</v>
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>1336</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>1147</v>
+        <v>1181</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>79</v>
+        <v>1183</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>339</v>
+        <v>1201</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>176</v>
+        <v>1207</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>164</v>
+        <v>1208</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>212</v>
+        <v>1209</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>947</v>
+        <v>1210</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>251</v>
+        <v>1206</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>295</v>
+        <v>1204</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>1033</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>1148</v>
+        <v>1182</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>80</v>
+        <v>1184</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>340</v>
+        <v>1200</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>177</v>
+        <v>1199</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>165</v>
+        <v>1213</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>213</v>
+        <v>1212</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>948</v>
+        <v>1211</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>252</v>
+        <v>1205</v>
       </c>
       <c r="I127" s="2" t="s">
-        <v>296</v>
+        <v>1203</v>
       </c>
       <c r="J127" s="2" t="s">
-        <v>1034</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>1149</v>
+        <v>1186</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>47</v>
+        <v>1185</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>358</v>
+        <v>1276</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>359</v>
+        <v>1272</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>360</v>
+        <v>1275</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>361</v>
+        <v>1283</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>907</v>
+        <v>1282</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>851</v>
+        <v>1281</v>
       </c>
       <c r="I128" s="2" t="s">
-        <v>263</v>
+        <v>1284</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>999</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>1150</v>
+        <v>1321</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>712</v>
+        <v>1320</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>853</v>
+        <v>1277</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>847</v>
+        <v>1273</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>848</v>
+        <v>1274</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>849</v>
+        <v>1278</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>949</v>
+        <v>1279</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>850</v>
+        <v>1280</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>852</v>
+        <v>1287</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>1035</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>713</v>
+        <v>1157</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>854</v>
+        <v>648</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>859</v>
+        <v>651</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>858</v>
+        <v>670</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>857</v>
+        <v>697</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>856</v>
+        <v>655</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>855</v>
+        <v>700</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>1036</v>
+        <v>452</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>714</v>
+        <v>1158</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>865</v>
+        <v>322</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>860</v>
+        <v>106</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>861</v>
+        <v>1319</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>862</v>
+        <v>198</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>951</v>
+        <v>925</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>863</v>
+        <v>234</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>864</v>
+        <v>279</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>1037</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>1171</v>
+        <v>1159</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>1170</v>
+        <v>1161</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>1190</v>
+        <v>1222</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>1191</v>
+        <v>1223</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>1192</v>
+        <v>1214</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>1193</v>
+        <v>1218</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>1194</v>
+        <v>1215</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>1195</v>
+        <v>1223</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>1196</v>
+        <v>1226</v>
       </c>
       <c r="J132" s="2" t="s">
-        <v>1197</v>
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>1216</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I133" s="2" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>1228</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>455</v>
+        <v>1164</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>452</v>
+        <v>1167</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>648</v>
+        <v>1242</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>651</v>
+        <v>1243</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>670</v>
+        <v>1238</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>697</v>
+        <v>1237</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>953</v>
+        <v>1236</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>655</v>
+        <v>1230</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>700</v>
+        <v>1231</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>452</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>456</v>
+        <v>1165</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>0</v>
+        <v>1168</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>320</v>
+        <v>1241</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>105</v>
+        <v>1244</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>146</v>
+        <v>1239</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>924</v>
+        <v>1240</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>1235</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>105</v>
+        <v>1233</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>278</v>
+        <v>1232</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>1014</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>457</v>
+        <v>1166</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>52</v>
+        <v>1187</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>318</v>
+        <v>1190</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>103</v>
+        <v>1191</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>144</v>
+        <v>1192</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>196</v>
+        <v>1193</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>922</v>
+        <v>1194</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>232</v>
+        <v>1195</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>276</v>
+        <v>1196</v>
       </c>
       <c r="J136" s="2" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="G137" s="2" t="s">
-        <v>954</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="I137" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="J137" s="2" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>923</v>
-      </c>
-      <c r="H138" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="I138" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="J138" s="2" t="s">
-        <v>1013</v>
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>460</v>
+        <v>1188</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>454</v>
+        <v>1189</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>650</v>
+        <v>1297</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>653</v>
+        <v>1296</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>672</v>
+        <v>1295</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>686</v>
+        <v>1298</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>955</v>
+        <v>1282</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>657</v>
+        <v>1299</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>701</v>
+        <v>1300</v>
       </c>
       <c r="J139" s="2" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="H140" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="I140" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="J140" s="2" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G141" s="2" t="s">
-        <v>926</v>
-      </c>
-      <c r="H141" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="J141" s="2" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>715</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="G142" s="2" t="s">
-        <v>927</v>
-      </c>
-      <c r="H142" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="I142" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="J142" s="2" t="s">
-        <v>1017</v>
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>1323</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>1335</v>
+        <v>1139</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>1180</v>
+        <v>75</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>1311</v>
+        <v>335</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>1312</v>
+        <v>174</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>1313</v>
+        <v>160</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>1314</v>
+        <v>208</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>1315</v>
+        <v>939</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>1316</v>
+        <v>247</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>1317</v>
+        <v>291</v>
       </c>
       <c r="J143" s="2" t="s">
-        <v>1318</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>1172</v>
+        <v>1140</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>1170</v>
+        <v>76</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>1190</v>
+        <v>336</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>1191</v>
+        <v>175</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>1192</v>
+        <v>161</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>1193</v>
+        <v>209</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>1194</v>
+        <v>940</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>1195</v>
+        <v>248</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>1196</v>
+        <v>292</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>1197</v>
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="I145" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>711</v>
+        <v>1142</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>452</v>
+        <v>377</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>648</v>
+        <v>628</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>651</v>
+        <v>627</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>670</v>
+        <v>626</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>697</v>
+        <v>625</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>953</v>
+        <v>942</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>655</v>
+        <v>624</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>700</v>
+        <v>623</v>
       </c>
       <c r="J146" s="2" t="s">
-        <v>452</v>
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I147" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J147" s="2" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>475</v>
+        <v>1144</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>53</v>
+        <v>375</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>319</v>
+        <v>647</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>104</v>
+        <v>640</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>145</v>
+        <v>641</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>197</v>
+        <v>639</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>923</v>
+        <v>944</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>233</v>
+        <v>638</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>277</v>
+        <v>637</v>
       </c>
       <c r="J148" s="2" t="s">
-        <v>1058</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>476</v>
+        <v>1145</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>56</v>
+        <v>376</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>323</v>
+        <v>646</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>107</v>
+        <v>643</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>149</v>
+        <v>642</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>199</v>
+        <v>644</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>926</v>
+        <v>945</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>235</v>
+        <v>645</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>280</v>
+        <v>636</v>
       </c>
       <c r="J149" s="2" t="s">
-        <v>1016</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>477</v>
+        <v>1146</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>925</v>
+        <v>946</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>1015</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>492</v>
+        <v>1147</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>927</v>
+        <v>947</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>1017</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>478</v>
+        <v>1148</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>103</v>
+        <v>177</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>922</v>
+        <v>948</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="J152" s="2" t="s">
-        <v>1012</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>1162</v>
+        <v>1149</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>1163</v>
+        <v>47</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>98</v>
+        <v>359</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>139</v>
+        <v>360</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>191</v>
+        <v>361</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>228</v>
+        <v>851</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="J153" s="2" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>479</v>
+        <v>1150</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>453</v>
+        <v>712</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>649</v>
+        <v>853</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>654</v>
+        <v>847</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>671</v>
+        <v>848</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>685</v>
+        <v>849</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>956</v>
+        <v>949</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>656</v>
+        <v>850</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>622</v>
+        <v>852</v>
       </c>
       <c r="J154" s="2" t="s">
-        <v>1057</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>480</v>
+        <v>1151</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>463</v>
+        <v>713</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>748</v>
+        <v>854</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>772</v>
+        <v>859</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>684</v>
+        <v>858</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>687</v>
+        <v>857</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>957</v>
+        <v>950</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>658</v>
+        <v>856</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>844</v>
+        <v>855</v>
       </c>
       <c r="J155" s="2" t="s">
-        <v>1083</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>481</v>
+        <v>1152</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>464</v>
+        <v>714</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>773</v>
+        <v>860</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>683</v>
+        <v>861</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>698</v>
+        <v>862</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>958</v>
+        <v>951</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>662</v>
+        <v>863</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>845</v>
+        <v>864</v>
       </c>
       <c r="J156" s="2" t="s">
-        <v>1084</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>482</v>
+        <v>1171</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>465</v>
+        <v>1170</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>755</v>
+        <v>1190</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>774</v>
+        <v>1191</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>682</v>
+        <v>1192</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>699</v>
+        <v>1193</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>959</v>
+        <v>1194</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>661</v>
+        <v>1195</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>846</v>
+        <v>1196</v>
       </c>
       <c r="J157" s="2" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>783</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="G158" s="2" t="s">
-        <v>960</v>
-      </c>
-      <c r="H158" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="I158" s="2" t="s">
-        <v>702</v>
-      </c>
-      <c r="J158" s="2" t="s">
-        <v>1074</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>484</v>
+        <v>455</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>757</v>
+        <v>648</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>775</v>
+        <v>651</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>689</v>
+        <v>697</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>1094</v>
+        <v>953</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="J159" s="2" t="s">
-        <v>1075</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>485</v>
+        <v>456</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>468</v>
+        <v>0</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>749</v>
+        <v>320</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>776</v>
+        <v>105</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>675</v>
+        <v>146</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>690</v>
+        <v>105</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>1095</v>
+        <v>924</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>660</v>
+        <v>105</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>704</v>
+        <v>278</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>1076</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>486</v>
+        <v>457</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>469</v>
+        <v>52</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>758</v>
+        <v>318</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>777</v>
+        <v>103</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>676</v>
+        <v>144</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>691</v>
+        <v>196</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>961</v>
+        <v>922</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>664</v>
+        <v>232</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>706</v>
+        <v>276</v>
       </c>
       <c r="J161" s="2" t="s">
-        <v>1080</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>487</v>
+        <v>458</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>750</v>
+        <v>649</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>778</v>
+        <v>652</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>707</v>
+        <v>622</v>
       </c>
       <c r="J162" s="2" t="s">
-        <v>1081</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>488</v>
+        <v>459</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>471</v>
+        <v>53</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>759</v>
+        <v>319</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>779</v>
+        <v>104</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>678</v>
+        <v>145</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>693</v>
+        <v>197</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>963</v>
+        <v>923</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>666</v>
+        <v>233</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>705</v>
+        <v>277</v>
       </c>
       <c r="J163" s="2" t="s">
-        <v>1077</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>489</v>
+        <v>460</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>760</v>
+        <v>650</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>780</v>
+        <v>653</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>964</v>
+        <v>955</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="J164" s="2" t="s">
-        <v>1078</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>490</v>
+        <v>461</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>473</v>
+        <v>55</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>761</v>
+        <v>322</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>781</v>
+        <v>106</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>680</v>
+        <v>148</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>695</v>
+        <v>198</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>965</v>
+        <v>925</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>668</v>
+        <v>234</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>709</v>
+        <v>279</v>
       </c>
       <c r="J165" s="2" t="s">
-        <v>1082</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>491</v>
+        <v>462</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>474</v>
+        <v>56</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>762</v>
+        <v>323</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>782</v>
+        <v>107</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>681</v>
+        <v>149</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>696</v>
+        <v>199</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>966</v>
+        <v>926</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>669</v>
+        <v>235</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>710</v>
+        <v>280</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>1079</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>736</v>
+        <v>57</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>751</v>
+        <v>324</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>784</v>
+        <v>108</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>796</v>
+        <v>150</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>808</v>
+        <v>200</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>967</v>
+        <v>927</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>820</v>
+        <v>236</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>832</v>
+        <v>281</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>1062</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>725</v>
+        <v>1335</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>737</v>
+        <v>1180</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>763</v>
+        <v>1311</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>785</v>
+        <v>1312</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>797</v>
+        <v>1313</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>809</v>
+        <v>1314</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>968</v>
+        <v>1315</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>821</v>
+        <v>1316</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>833</v>
+        <v>1317</v>
       </c>
       <c r="J168" s="2" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="s">
-        <v>726</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>738</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>764</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>786</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>798</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>810</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>969</v>
-      </c>
-      <c r="H169" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="I169" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="J169" s="2" t="s">
-        <v>1064</v>
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>1362</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>727</v>
+        <v>1172</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>739</v>
+        <v>1170</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>765</v>
+        <v>1190</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>795</v>
+        <v>1191</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>799</v>
+        <v>1192</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>811</v>
+        <v>1193</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>1097</v>
+        <v>1194</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>823</v>
+        <v>1195</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>835</v>
+        <v>1196</v>
       </c>
       <c r="J170" s="2" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>787</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="F171" s="2" t="s">
-        <v>812</v>
-      </c>
-      <c r="G171" s="2" t="s">
-        <v>1096</v>
-      </c>
-      <c r="H171" s="2" t="s">
-        <v>824</v>
-      </c>
-      <c r="I171" s="2" t="s">
-        <v>836</v>
-      </c>
-      <c r="J171" s="2" t="s">
-        <v>1066</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>729</v>
+        <v>711</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>741</v>
+        <v>452</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>752</v>
+        <v>648</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>788</v>
+        <v>651</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>801</v>
+        <v>670</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>813</v>
+        <v>697</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>1098</v>
+        <v>953</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>825</v>
+        <v>655</v>
       </c>
       <c r="I172" s="2" t="s">
-        <v>837</v>
+        <v>700</v>
       </c>
       <c r="J172" s="2" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>730</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>742</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="E173" s="2" t="s">
-        <v>802</v>
-      </c>
-      <c r="F173" s="2" t="s">
-        <v>814</v>
-      </c>
-      <c r="G173" s="2" t="s">
-        <v>970</v>
-      </c>
-      <c r="H173" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="I173" s="2" t="s">
-        <v>838</v>
-      </c>
-      <c r="J173" s="2" t="s">
-        <v>1068</v>
+        <v>452</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>731</v>
+        <v>475</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>743</v>
+        <v>53</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>753</v>
+        <v>319</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>790</v>
+        <v>104</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>803</v>
+        <v>145</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>815</v>
+        <v>197</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>971</v>
+        <v>923</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>827</v>
+        <v>233</v>
       </c>
       <c r="I174" s="2" t="s">
-        <v>839</v>
+        <v>277</v>
       </c>
       <c r="J174" s="2" t="s">
-        <v>1069</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>732</v>
+        <v>476</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>744</v>
+        <v>56</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>768</v>
+        <v>323</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>791</v>
+        <v>107</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>804</v>
+        <v>149</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>816</v>
+        <v>199</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>972</v>
+        <v>926</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>828</v>
+        <v>235</v>
       </c>
       <c r="I175" s="2" t="s">
-        <v>840</v>
+        <v>280</v>
       </c>
       <c r="J175" s="2" t="s">
-        <v>1070</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>733</v>
+        <v>477</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>745</v>
+        <v>55</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>769</v>
+        <v>322</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>792</v>
+        <v>106</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>805</v>
+        <v>148</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>817</v>
+        <v>198</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>973</v>
+        <v>925</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>829</v>
+        <v>234</v>
       </c>
       <c r="I176" s="2" t="s">
-        <v>841</v>
+        <v>279</v>
       </c>
       <c r="J176" s="2" t="s">
-        <v>1071</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>734</v>
+        <v>492</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>746</v>
+        <v>57</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>770</v>
+        <v>324</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>793</v>
+        <v>108</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>806</v>
+        <v>150</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>818</v>
+        <v>200</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>974</v>
+        <v>927</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>830</v>
+        <v>236</v>
       </c>
       <c r="I177" s="2" t="s">
-        <v>842</v>
+        <v>281</v>
       </c>
       <c r="J177" s="2" t="s">
-        <v>1072</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>735</v>
+        <v>478</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>747</v>
+        <v>52</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>771</v>
+        <v>318</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>794</v>
+        <v>103</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>807</v>
+        <v>144</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>819</v>
+        <v>196</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>975</v>
+        <v>922</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>831</v>
+        <v>232</v>
       </c>
       <c r="I178" s="2" t="s">
-        <v>843</v>
+        <v>276</v>
       </c>
       <c r="J178" s="2" t="s">
-        <v>1073</v>
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G179" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="H179" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I179" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="J179" s="2" t="s">
+        <v>1007</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>1121</v>
+        <v>479</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>1125</v>
+        <v>453</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>1246</v>
+        <v>649</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>1245</v>
+        <v>654</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>1125</v>
+        <v>671</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>1263</v>
+        <v>685</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>1262</v>
+        <v>956</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>1245</v>
+        <v>656</v>
       </c>
       <c r="I180" s="2" t="s">
-        <v>1264</v>
+        <v>622</v>
       </c>
       <c r="J180" s="2" t="s">
-        <v>1265</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>1122</v>
+        <v>480</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>1126</v>
+        <v>463</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>1248</v>
+        <v>748</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>1249</v>
+        <v>772</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>1247</v>
+        <v>684</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>1259</v>
+        <v>687</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>1260</v>
+        <v>957</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>1261</v>
+        <v>658</v>
       </c>
       <c r="I181" s="2" t="s">
-        <v>1271</v>
+        <v>844</v>
       </c>
       <c r="J181" s="2" t="s">
-        <v>1270</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>1123</v>
+        <v>481</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>1127</v>
+        <v>464</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>1251</v>
+        <v>754</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>1250</v>
+        <v>773</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>1252</v>
+        <v>683</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>1257</v>
+        <v>698</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>1258</v>
+        <v>958</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>1250</v>
+        <v>662</v>
       </c>
       <c r="I182" s="2" t="s">
-        <v>1268</v>
+        <v>845</v>
       </c>
       <c r="J182" s="2" t="s">
-        <v>1269</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>1124</v>
+        <v>482</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>1128</v>
+        <v>465</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>1255</v>
+        <v>755</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>1254</v>
+        <v>774</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>1253</v>
+        <v>682</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>1254</v>
+        <v>699</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>1256</v>
+        <v>959</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>1254</v>
+        <v>661</v>
       </c>
       <c r="I183" s="2" t="s">
-        <v>1267</v>
+        <v>846</v>
       </c>
       <c r="J183" s="2" t="s">
-        <v>1266</v>
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="G184" s="2" t="s">
+        <v>960</v>
+      </c>
+      <c r="H184" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="I184" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="J184" s="2" t="s">
+        <v>1074</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>40</v>
+        <v>484</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>82</v>
+        <v>467</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>309</v>
+        <v>757</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>120</v>
+        <v>775</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>133</v>
+        <v>674</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>185</v>
+        <v>689</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>911</v>
+        <v>1094</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>226</v>
+        <v>663</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>265</v>
+        <v>703</v>
       </c>
       <c r="J185" s="2" t="s">
-        <v>1003</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>38</v>
+        <v>485</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>84</v>
+        <v>468</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>84</v>
+        <v>749</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>122</v>
+        <v>776</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>84</v>
+        <v>675</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>215</v>
+        <v>690</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>976</v>
+        <v>1095</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>253</v>
+        <v>660</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>298</v>
+        <v>704</v>
       </c>
       <c r="J186" s="2" t="s">
-        <v>1040</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>39</v>
+        <v>486</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>85</v>
+        <v>469</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>342</v>
+        <v>758</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>123</v>
+        <v>777</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>167</v>
+        <v>676</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>216</v>
+        <v>691</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>977</v>
+        <v>961</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>254</v>
+        <v>664</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>299</v>
+        <v>706</v>
       </c>
       <c r="J187" s="2" t="s">
-        <v>1041</v>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="G188" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="H188" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="I188" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="J188" s="2" t="s">
+        <v>1081</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>41</v>
+        <v>488</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>86</v>
+        <v>471</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>343</v>
+        <v>759</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>124</v>
+        <v>779</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>168</v>
+        <v>678</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>217</v>
+        <v>693</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>978</v>
+        <v>963</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>255</v>
+        <v>666</v>
       </c>
       <c r="I189" s="2" t="s">
-        <v>300</v>
+        <v>705</v>
       </c>
       <c r="J189" s="2" t="s">
-        <v>1042</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="G190" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="H190" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="I190" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="J190" s="2" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="H191" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="I191" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="J191" s="2" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="G192" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="H192" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="I192" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="J192" s="2" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="G193" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="H193" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="I193" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="J193" s="2" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="G194" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="H194" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="I194" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="J194" s="2" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="G195" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="H195" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="I195" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="J195" s="2" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="G196" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="I196" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="J196" s="2" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>1096</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="I197" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="J197" s="2" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="F198" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="G198" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="H198" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="I198" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="J198" s="2" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="G199" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="I199" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="J199" s="2" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F200" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="I200" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="J200" s="2" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="H201" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="I201" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="J201" s="2" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="F202" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="H202" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="I202" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="J202" s="2" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="I203" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="J203" s="2" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="G204" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="H204" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="I204" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="J204" s="2" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F206" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>1262</v>
+      </c>
+      <c r="H206" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="I206" s="2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="J206" s="2" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>1249</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>1260</v>
+      </c>
+      <c r="H207" s="2" t="s">
+        <v>1261</v>
+      </c>
+      <c r="I207" s="2" t="s">
+        <v>1271</v>
+      </c>
+      <c r="J207" s="2" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="I208" s="2" t="s">
+        <v>1268</v>
+      </c>
+      <c r="J208" s="2" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H209" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="I209" s="2" t="s">
+        <v>1267</v>
+      </c>
+      <c r="J209" s="2" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="H211" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I211" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="J211" s="2" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G212" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="H212" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I212" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="J212" s="2" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G213" s="2" t="s">
+        <v>977</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="I213" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J213" s="2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G215" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I215" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="J215" s="2" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B216" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C216" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D190" s="2" t="s">
+      <c r="D216" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E190" s="2" t="s">
+      <c r="E216" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F190" s="2" t="s">
+      <c r="F216" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G190" s="2" t="s">
+      <c r="G216" s="2" t="s">
         <v>979</v>
       </c>
-      <c r="H190" s="2" t="s">
+      <c r="H216" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="I190" s="2" t="s">
+      <c r="I216" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J190" s="2" t="s">
+      <c r="J216" s="2" t="s">
         <v>1043</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- V 0.91.08; Debugging and issues fixed 	- DeviceIABP: color scheme visibility re: buttons 	- DeviceDefib: toggling into defib mode from pacer/sync; also added defib mode button 	- DeviceMonitor: Cap moved from 5 numerics/tracings to 9 numerics and 8 tracings
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE70273-9654-4CC0-941C-E69EA0FAA313}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5775BC60-B142-4779-B53A-F55042FBB3F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4041,9 +4041,6 @@
     <t>IABP:Helium</t>
   </si>
   <si>
-    <t>DEFIB:On</t>
-  </si>
-  <si>
     <t>DEFIB:WindowTitle</t>
   </si>
   <si>
@@ -4177,6 +4174,9 @@
   </si>
   <si>
     <t>DEFIB:Milliamps</t>
+  </si>
+  <si>
+    <t>DEFIB:Defibrillator</t>
   </si>
 </sst>
 </file>
@@ -4543,7 +4543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B111" sqref="B111"/>
+      <selection pane="topRight" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7010,103 +7010,103 @@
     </row>
     <row r="95" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>1339</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="97" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>1338</v>
+        <v>1383</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1177</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>1353</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>1354</v>
       </c>
     </row>
     <row r="101" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="102" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="103" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="105" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="106" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="107" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="108" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>1168</v>
@@ -7114,82 +7114,82 @@
     </row>
     <row r="109" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="110" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="111" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>1369</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>1370</v>
       </c>
     </row>
     <row r="112" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="113" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="114" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="115" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="116" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="117" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="118" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>1380</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>1381</v>
       </c>
     </row>
     <row r="120" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8506,10 +8506,10 @@
     </row>
     <row r="169" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- V 0.93.07; Versioning updates; Defibrillation and Pacemaker updates   - StatusBar on PatientEditor shows if version update available (Issue #31)     - Strings localized to all languages   - Tidied up "To Do.md" into "Notes.md", moved to-do list to Github issues   - Defibrillation waveform narrowed, removed post-shock pause (Issue #32)   - Pacemaker functionality (Issue #32):     - Modeled in Patient, timer functioning appropriately 	- Triggers pacemaker spike, overwrites waveform on strip appropriately 	- Paced beats (energy > threshold) resets cardiac baseline timer (overrides native heart node timing) 	  - Paced beats marked as aberrant and display as such (slightly wide QRS, deflects abnormally) 	- Pacemaker values included in Save/Load   - Known issues:     - Strip.cs x-axis intervals (draw resolution) too large/low, causes choppy waveforms 	- Need to add Pacer energy threshold to PatientEditor
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117E5617-AF8A-4CB5-9DE8-C914E20D1946}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02EB216-2E2E-4EC4-A589-2EC516E51B1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6750" uniqueCount="2625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="2641">
   <si>
     <t>Temperature</t>
   </si>
@@ -7900,6 +7900,54 @@
   </si>
   <si>
     <t>Sélectionnez la langue et les conditions d'utilisation</t>
+  </si>
+  <si>
+    <t>STATUS:UpdateAvailable</t>
+  </si>
+  <si>
+    <t>Infirmary Integrated needs updating. Click here for version {0}</t>
+  </si>
+  <si>
+    <t>Le programme doit être mis à jour. Cliquez ici pour la version {0}</t>
+  </si>
+  <si>
+    <t>El programa necesita ser actualizado. Haga clic aquí para la versión {0}</t>
+  </si>
+  <si>
+    <t>برنامه باید به روز شود. اینجا کلیک کنید برای نسخه {0}</t>
+  </si>
+  <si>
+    <t>Das Programm muss aktualisiert werden. Klicken Sie hier für Version {0}</t>
+  </si>
+  <si>
+    <t>该程序需要更新。 单击此处查看版本{0}</t>
+  </si>
+  <si>
+    <t>يحتاج البرنامج إلى التحديث. انقر هنا للحصول على الإصدار {0}</t>
+  </si>
+  <si>
+    <t>ፕሮግራሙ መዘመን ያስፈልገዋል. ለዚህ እትም {0} ጠቅ ያድርጉ</t>
+  </si>
+  <si>
+    <t>יש לעדכן את התוכנית. לחץ כאן לגרסה {0}</t>
+  </si>
+  <si>
+    <t>कार्यक्रम को अद्यतन करने की आवश्यकता है। संस्करण {0} के लिए यहां क्लिक करें</t>
+  </si>
+  <si>
+    <t>Il programma deve essere aggiornato. Clicca qui per la versione {0}</t>
+  </si>
+  <si>
+    <t>프로그램을 업데이트해야합니다. 버전 {0}을 보려면 여기를 클릭하십시오.</t>
+  </si>
+  <si>
+    <t>O programa precisa ser atualizado. Clique aqui para a versão {0}</t>
+  </si>
+  <si>
+    <t>Программа должна быть обновлена. Нажмите здесь для версии {0}</t>
+  </si>
+  <si>
+    <t>Mpango huo unahitaji kubadilishwa. Bofya hapa kwa toleo {0}</t>
   </si>
 </sst>
 </file>
@@ -8271,11 +8319,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P225"/>
+  <dimension ref="A1:P227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B222" sqref="B222"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A219" sqref="A219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17924,302 +17972,353 @@
     <row r="218" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="219" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
-        <v>40</v>
+        <v>2625</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>80</v>
+        <v>2626</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>1603</v>
+        <v>2633</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>1829</v>
+        <v>2632</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>2404</v>
+        <v>2631</v>
       </c>
       <c r="F219" s="4" t="s">
-        <v>301</v>
+        <v>2630</v>
       </c>
       <c r="G219" s="4" t="s">
-        <v>1838</v>
+        <v>2629</v>
       </c>
       <c r="H219" s="4" t="s">
-        <v>117</v>
+        <v>2628</v>
       </c>
       <c r="I219" s="4" t="s">
-        <v>129</v>
+        <v>2627</v>
       </c>
       <c r="J219" s="4" t="s">
-        <v>1945</v>
+        <v>2634</v>
       </c>
       <c r="K219" s="4" t="s">
-        <v>2406</v>
+        <v>2635</v>
       </c>
       <c r="L219" s="4" t="s">
-        <v>180</v>
+        <v>2636</v>
       </c>
       <c r="M219" s="4" t="s">
-        <v>898</v>
+        <v>2637</v>
       </c>
       <c r="N219" s="4" t="s">
-        <v>220</v>
+        <v>2638</v>
       </c>
       <c r="O219" s="4" t="s">
-        <v>258</v>
+        <v>2639</v>
       </c>
       <c r="P219" s="4" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="220" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B220" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C220" s="4" t="s">
-        <v>1680</v>
-      </c>
-      <c r="D220" s="4" t="s">
-        <v>1943</v>
-      </c>
-      <c r="E220" s="4" t="s">
-        <v>2405</v>
-      </c>
-      <c r="F220" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G220" s="4" t="s">
-        <v>1944</v>
-      </c>
-      <c r="H220" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I220" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J220" s="4" t="s">
-        <v>1946</v>
-      </c>
-      <c r="K220" s="4" t="s">
-        <v>2407</v>
-      </c>
-      <c r="L220" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="M220" s="4" t="s">
-        <v>963</v>
-      </c>
-      <c r="N220" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="O220" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="P220" s="4" t="s">
-        <v>1026</v>
-      </c>
-    </row>
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="221" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>1681</v>
+        <v>1603</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>1948</v>
+        <v>1829</v>
       </c>
       <c r="E221" s="4" t="s">
-        <v>2409</v>
+        <v>2404</v>
       </c>
       <c r="F221" s="4" t="s">
-        <v>334</v>
+        <v>301</v>
       </c>
       <c r="G221" s="4" t="s">
-        <v>1949</v>
+        <v>1838</v>
       </c>
       <c r="H221" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I221" s="4" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="J221" s="4" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="K221" s="4" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="L221" s="4" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="M221" s="4" t="s">
-        <v>964</v>
+        <v>898</v>
       </c>
       <c r="N221" s="4" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="O221" s="4" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="P221" s="4" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="222" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>989</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>1943</v>
+      </c>
+      <c r="E222" s="4" t="s">
+        <v>2405</v>
+      </c>
+      <c r="F222" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G222" s="4" t="s">
+        <v>1944</v>
+      </c>
+      <c r="H222" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I222" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J222" s="4" t="s">
+        <v>1946</v>
+      </c>
+      <c r="K222" s="4" t="s">
+        <v>2407</v>
+      </c>
+      <c r="L222" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="M222" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="N222" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="O222" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="P222" s="4" t="s">
+        <v>1026</v>
+      </c>
+    </row>
     <row r="223" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
-        <v>2593</v>
+        <v>39</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>2595</v>
+        <v>83</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>2597</v>
+        <v>1681</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>2619</v>
+        <v>1948</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>2620</v>
+        <v>2409</v>
       </c>
       <c r="F223" s="4" t="s">
-        <v>2621</v>
+        <v>334</v>
       </c>
       <c r="G223" s="4" t="s">
-        <v>2622</v>
+        <v>1949</v>
       </c>
       <c r="H223" s="4" t="s">
-        <v>2623</v>
+        <v>120</v>
       </c>
       <c r="I223" s="4" t="s">
-        <v>2624</v>
+        <v>163</v>
       </c>
       <c r="J223" s="4" t="s">
-        <v>2618</v>
+        <v>1947</v>
       </c>
       <c r="K223" s="4" t="s">
-        <v>2617</v>
+        <v>2408</v>
       </c>
       <c r="L223" s="4" t="s">
-        <v>2616</v>
+        <v>211</v>
       </c>
       <c r="M223" s="4" t="s">
-        <v>2615</v>
+        <v>964</v>
       </c>
       <c r="N223" s="4" t="s">
-        <v>2614</v>
+        <v>248</v>
       </c>
       <c r="O223" s="4" t="s">
-        <v>2613</v>
+        <v>292</v>
       </c>
       <c r="P223" s="4" t="s">
-        <v>2612</v>
-      </c>
-    </row>
-    <row r="224" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="4" t="s">
-        <v>2592</v>
-      </c>
-      <c r="B224" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C224" s="4" t="s">
-        <v>1679</v>
-      </c>
-      <c r="D224" s="4" t="s">
-        <v>1950</v>
-      </c>
-      <c r="E224" s="4" t="s">
-        <v>2410</v>
-      </c>
-      <c r="F224" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="G224" s="4" t="s">
-        <v>1951</v>
-      </c>
-      <c r="H224" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I224" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="J224" s="4" t="s">
-        <v>1952</v>
-      </c>
-      <c r="K224" s="4" t="s">
-        <v>2411</v>
-      </c>
-      <c r="L224" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="M224" s="4" t="s">
-        <v>965</v>
-      </c>
-      <c r="N224" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="O224" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="P224" s="4" t="s">
-        <v>1028</v>
-      </c>
-    </row>
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="225" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
+        <v>2593</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>2595</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>2597</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>2619</v>
+      </c>
+      <c r="E225" s="4" t="s">
+        <v>2620</v>
+      </c>
+      <c r="F225" s="4" t="s">
+        <v>2621</v>
+      </c>
+      <c r="G225" s="4" t="s">
+        <v>2622</v>
+      </c>
+      <c r="H225" s="4" t="s">
+        <v>2623</v>
+      </c>
+      <c r="I225" s="4" t="s">
+        <v>2624</v>
+      </c>
+      <c r="J225" s="4" t="s">
+        <v>2618</v>
+      </c>
+      <c r="K225" s="4" t="s">
+        <v>2617</v>
+      </c>
+      <c r="L225" s="4" t="s">
+        <v>2616</v>
+      </c>
+      <c r="M225" s="4" t="s">
+        <v>2615</v>
+      </c>
+      <c r="N225" s="4" t="s">
+        <v>2614</v>
+      </c>
+      <c r="O225" s="4" t="s">
+        <v>2613</v>
+      </c>
+      <c r="P225" s="4" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="4" t="s">
+        <v>2592</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>1679</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>1950</v>
+      </c>
+      <c r="E226" s="4" t="s">
+        <v>2410</v>
+      </c>
+      <c r="F226" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="G226" s="4" t="s">
+        <v>1951</v>
+      </c>
+      <c r="H226" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I226" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="J226" s="4" t="s">
+        <v>1952</v>
+      </c>
+      <c r="K226" s="4" t="s">
+        <v>2411</v>
+      </c>
+      <c r="L226" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="M226" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="N226" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="O226" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="P226" s="4" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="4" t="s">
         <v>2594</v>
       </c>
-      <c r="B225" s="4" t="s">
+      <c r="B227" s="4" t="s">
         <v>2596</v>
       </c>
-      <c r="C225" s="4" t="s">
+      <c r="C227" s="4" t="s">
         <v>2598</v>
       </c>
-      <c r="D225" s="4" t="s">
+      <c r="D227" s="4" t="s">
         <v>2599</v>
       </c>
-      <c r="E225" s="4" t="s">
+      <c r="E227" s="4" t="s">
         <v>2600</v>
       </c>
-      <c r="F225" s="4" t="s">
+      <c r="F227" s="4" t="s">
         <v>2601</v>
       </c>
-      <c r="G225" s="4" t="s">
+      <c r="G227" s="4" t="s">
         <v>2602</v>
       </c>
-      <c r="H225" s="5" t="s">
+      <c r="H227" s="5" t="s">
         <v>2603</v>
       </c>
-      <c r="I225" s="4" t="s">
+      <c r="I227" s="4" t="s">
         <v>2604</v>
       </c>
-      <c r="J225" s="4" t="s">
+      <c r="J227" s="4" t="s">
         <v>2605</v>
       </c>
-      <c r="K225" s="4" t="s">
+      <c r="K227" s="4" t="s">
         <v>2606</v>
       </c>
-      <c r="L225" s="4" t="s">
+      <c r="L227" s="4" t="s">
         <v>2607</v>
       </c>
-      <c r="M225" s="4" t="s">
+      <c r="M227" s="4" t="s">
         <v>2608</v>
       </c>
-      <c r="N225" s="4" t="s">
+      <c r="N227" s="4" t="s">
         <v>2609</v>
       </c>
-      <c r="O225" s="4" t="s">
+      <c r="O227" s="4" t="s">
         <v>2610</v>
       </c>
-      <c r="P225" s="4" t="s">
+      <c r="P227" s="4" t="s">
         <v>2611</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- V 0.97 Release; Localization updated
</commit_message>
<xml_diff>
--- a/II_Core/Localization Strings.xlsx
+++ b/II_Core/Localization Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibi\Documents\Infirmary Integrated\II_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB38BE38-D714-40F7-9964-90B45BD6A4B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C104556F-03A2-4283-83C8-C7CCC93DD095}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="203" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="2683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6814" uniqueCount="2851">
   <si>
     <t>Temperature</t>
   </si>
@@ -8074,6 +8074,510 @@
   </si>
   <si>
     <t>Patient Parameters Reset</t>
+  </si>
+  <si>
+    <t>Spiegel Patientendaten</t>
+  </si>
+  <si>
+    <t>Klient</t>
+  </si>
+  <si>
+    <t>Zugangsschlüssel</t>
+  </si>
+  <si>
+    <t>Zugangspasswort</t>
+  </si>
+  <si>
+    <t>Administrator-Passwort</t>
+  </si>
+  <si>
+    <t>Spiegelungsfunktion aktiviert</t>
+  </si>
+  <si>
+    <t>Patientenparameter aktualisiert</t>
+  </si>
+  <si>
+    <t>Reflektierte Patientenparameter aktualisiert</t>
+  </si>
+  <si>
+    <t>Patientenparameter zurücksetzen</t>
+  </si>
+  <si>
+    <t>Spiegelungsfunktion Behinderte</t>
+  </si>
+  <si>
+    <t>Datos del Paciente espejo</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Llave de acceso</t>
+  </si>
+  <si>
+    <t>Contraseña de acceso</t>
+  </si>
+  <si>
+    <t>La duplicación se Activado</t>
+  </si>
+  <si>
+    <t>Duplicación de movilidad reducida</t>
+  </si>
+  <si>
+    <t>Actualizado parámetros del paciente</t>
+  </si>
+  <si>
+    <t>Restablecer los parámetros del paciente</t>
+  </si>
+  <si>
+    <t>Reflejo de los parámetros del paciente actualizado</t>
+  </si>
+  <si>
+    <t>Réflexion données patient</t>
+  </si>
+  <si>
+    <t>Statut</t>
+  </si>
+  <si>
+    <t>Serveur</t>
+  </si>
+  <si>
+    <t>Clé d'accès</t>
+  </si>
+  <si>
+    <t>Mot de passe pour l'accès</t>
+  </si>
+  <si>
+    <t>Mot de passe administrateur</t>
+  </si>
+  <si>
+    <t>Mise à jour des paramètres du patient</t>
+  </si>
+  <si>
+    <t>Paramètres du patient réinitialiser</t>
+  </si>
+  <si>
+    <t>Mise à jour des patients paramètres miroir</t>
+  </si>
+  <si>
+    <t>Réflexion désactivé</t>
+  </si>
+  <si>
+    <t>Réflexion activé</t>
+  </si>
+  <si>
+    <t>Riflessione dati paziente</t>
+  </si>
+  <si>
+    <t>Stato</t>
+  </si>
+  <si>
+    <t>Non attivo</t>
+  </si>
+  <si>
+    <t>Chiave di accesso</t>
+  </si>
+  <si>
+    <t>Password per l'accesso</t>
+  </si>
+  <si>
+    <t>Password dell'amministratore</t>
+  </si>
+  <si>
+    <t>Resettare i parametri del paziente</t>
+  </si>
+  <si>
+    <t>I parametri del paziente aggiornato</t>
+  </si>
+  <si>
+    <t>Mirroring parametri del paziente aggiornato</t>
+  </si>
+  <si>
+    <t>Riflessione disattivato</t>
+  </si>
+  <si>
+    <t>Riflessione attivato</t>
+  </si>
+  <si>
+    <t>Chave de acesso</t>
+  </si>
+  <si>
+    <t>Senha de acesso</t>
+  </si>
+  <si>
+    <t>Senha do administrador</t>
+  </si>
+  <si>
+    <t>Reflexão activado</t>
+  </si>
+  <si>
+    <t>Reflexão desativada</t>
+  </si>
+  <si>
+    <t>Parâmetros paciente atualizado</t>
+  </si>
+  <si>
+    <t>Espelhando os parâmetros do paciente atualizado</t>
+  </si>
+  <si>
+    <t>Parâmetros paciente repor</t>
+  </si>
+  <si>
+    <t>Dados do paciente reflexão</t>
+  </si>
+  <si>
+    <t>Отражение данных пациента</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>сервер</t>
+  </si>
+  <si>
+    <t>клиент</t>
+  </si>
+  <si>
+    <t>Ключ доступа</t>
+  </si>
+  <si>
+    <t>Пароль для доступа</t>
+  </si>
+  <si>
+    <t>Пароль администратора</t>
+  </si>
+  <si>
+    <t>Отражение активирован</t>
+  </si>
+  <si>
+    <t>Отражение отключена</t>
+  </si>
+  <si>
+    <t>Параметры пациента Обновлено</t>
+  </si>
+  <si>
+    <t>Зеркальные параметры пациента Обновлены</t>
+  </si>
+  <si>
+    <t>Параметры пациента Сброс</t>
+  </si>
+  <si>
+    <t>Tafakari Mgonjwa Data</t>
+  </si>
+  <si>
+    <t>Hali</t>
+  </si>
+  <si>
+    <t>Isiyotumika</t>
+  </si>
+  <si>
+    <t>Kupata muhimu</t>
+  </si>
+  <si>
+    <t>Mteja</t>
+  </si>
+  <si>
+    <t>Tafakari ulioamilishwa</t>
+  </si>
+  <si>
+    <t>Tafakari walemavu</t>
+  </si>
+  <si>
+    <t>Vigezo mgonjwa rudisha</t>
+  </si>
+  <si>
+    <t>Vipengele vya mgonjwa kusasishwa</t>
+  </si>
+  <si>
+    <t>Kuzingatia vigezo vya mgonjwa kusasishwa</t>
+  </si>
+  <si>
+    <t>Nenosiri la kupata</t>
+  </si>
+  <si>
+    <t>Nenosiri la msimamizi</t>
+  </si>
+  <si>
+    <t>Contraseña de administrador</t>
+  </si>
+  <si>
+    <t>Seva</t>
+  </si>
+  <si>
+    <t>반사 환자 데이터</t>
+  </si>
+  <si>
+    <t>지위</t>
+  </si>
+  <si>
+    <t>숙주</t>
+  </si>
+  <si>
+    <t>고객</t>
+  </si>
+  <si>
+    <t>액세스 키</t>
+  </si>
+  <si>
+    <t>액세스를위한 비밀번호</t>
+  </si>
+  <si>
+    <t>관리자 비밀번호</t>
+  </si>
+  <si>
+    <t>반사 활성화</t>
+  </si>
+  <si>
+    <t>반사 비활성화</t>
+  </si>
+  <si>
+    <t>환자 매개 변수 업데이트</t>
+  </si>
+  <si>
+    <t>업데이트 환자 매개 변수를 미러링</t>
+  </si>
+  <si>
+    <t>환자 매개 변수 재설정</t>
+  </si>
+  <si>
+    <t>डाटा रोगी के परावर्तन</t>
+  </si>
+  <si>
+    <t>वर्तमान स्थिति</t>
+  </si>
+  <si>
+    <t>निष्क्रिय</t>
+  </si>
+  <si>
+    <t>मेज़बान</t>
+  </si>
+  <si>
+    <t>ग्राहक</t>
+  </si>
+  <si>
+    <t>आगमन चाबी</t>
+  </si>
+  <si>
+    <t>उपयोग करने के लिए पासवर्ड</t>
+  </si>
+  <si>
+    <t>व्यवस्थापक का पारण शब्द</t>
+  </si>
+  <si>
+    <t>प्रतिबिंब सक्रिय</t>
+  </si>
+  <si>
+    <t>प्रतिबिंब अक्षम</t>
+  </si>
+  <si>
+    <t>रोगी पैरामीटर अपडेट किया गया</t>
+  </si>
+  <si>
+    <t>रोगी पैरामीटर अपडेट किया गया मिररिंग</t>
+  </si>
+  <si>
+    <t>रोगी पैरामीटर रीसेट</t>
+  </si>
+  <si>
+    <t>השתקפות של חולה נתונים</t>
+  </si>
+  <si>
+    <t>מצב</t>
+  </si>
+  <si>
+    <t>לא פעיל</t>
+  </si>
+  <si>
+    <t>מארח</t>
+  </si>
+  <si>
+    <t>לקוח</t>
+  </si>
+  <si>
+    <t>מפתח גישה</t>
+  </si>
+  <si>
+    <t>סיסמה עבור גישה</t>
+  </si>
+  <si>
+    <t>סיסמת מנהל</t>
+  </si>
+  <si>
+    <t>השתקפות מופעלת</t>
+  </si>
+  <si>
+    <t>השתקפות מושבת</t>
+  </si>
+  <si>
+    <t>עודכנו פרמטרים חולים</t>
+  </si>
+  <si>
+    <t>שיקוף פרמטרים חולים עודכנו</t>
+  </si>
+  <si>
+    <t>פרמטרים חולים איפוס</t>
+  </si>
+  <si>
+    <t>بازتاب بیمار داده</t>
+  </si>
+  <si>
+    <t>وضعیت</t>
+  </si>
+  <si>
+    <t>غیر فعال</t>
+  </si>
+  <si>
+    <t>میزبان</t>
+  </si>
+  <si>
+    <t>مشتری</t>
+  </si>
+  <si>
+    <t>کلید دسترسی</t>
+  </si>
+  <si>
+    <t>رمز عبور برای دسترسی</t>
+  </si>
+  <si>
+    <t>رمز عبور</t>
+  </si>
+  <si>
+    <t>بازتاب فعال</t>
+  </si>
+  <si>
+    <t>بازتاب غیر فعال</t>
+  </si>
+  <si>
+    <t>پارامترهای بیمار به روز رسانی</t>
+  </si>
+  <si>
+    <t>معکوس پارامترهای بیمار به روز رسانی</t>
+  </si>
+  <si>
+    <t>پارامترهای بیمار تنظیم مجدد</t>
+  </si>
+  <si>
+    <t>الحالة</t>
+  </si>
+  <si>
+    <t>غير نشط</t>
+  </si>
+  <si>
+    <t>مضيف</t>
+  </si>
+  <si>
+    <t>عميل</t>
+  </si>
+  <si>
+    <t>مفتاح الوصول</t>
+  </si>
+  <si>
+    <t>كلمة مرور للوصول</t>
+  </si>
+  <si>
+    <t>كلمة مرور المسؤول</t>
+  </si>
+  <si>
+    <t>انعكاس تفعيلها</t>
+  </si>
+  <si>
+    <t>انعكاس تعطيل</t>
+  </si>
+  <si>
+    <t>معلمات المريض التحديث</t>
+  </si>
+  <si>
+    <t>يعكس معلمات المرضى تحديث</t>
+  </si>
+  <si>
+    <t>معلمات المريض إعادة تعيين</t>
+  </si>
+  <si>
+    <t>انعكاس المريض البيانات</t>
+  </si>
+  <si>
+    <t>የውሂብ ሕመምተኞች መካከል ነጸብራቅ</t>
+  </si>
+  <si>
+    <t>ሁናቴ</t>
+  </si>
+  <si>
+    <t>የማይሠራ</t>
+  </si>
+  <si>
+    <t>አስተናጋጅ</t>
+  </si>
+  <si>
+    <t>ደምበኛ</t>
+  </si>
+  <si>
+    <t>የመዳረሻ ቁልፍ</t>
+  </si>
+  <si>
+    <t>መዳረሻ ለ የይለፍ ቃል</t>
+  </si>
+  <si>
+    <t>አስተዳዳሪ የይለፍ ቃል</t>
+  </si>
+  <si>
+    <t>ነፀብራቅ ገብሯል</t>
+  </si>
+  <si>
+    <t>ነፀብራቅ ተሰናክሏል</t>
+  </si>
+  <si>
+    <t>የታካሚ ግቤቶች ተሻሽለዋል</t>
+  </si>
+  <si>
+    <t>የታካሚ የታካሚ መለኪያዎች ተሻሽለዋል</t>
+  </si>
+  <si>
+    <t>የታካሚ መለኪያዎች ዳግም ማስጀመር</t>
+  </si>
+  <si>
+    <t>数据病人的反思</t>
+  </si>
+  <si>
+    <t>状态</t>
+  </si>
+  <si>
+    <t>待用</t>
+  </si>
+  <si>
+    <t>主办</t>
+  </si>
+  <si>
+    <t>客户</t>
+  </si>
+  <si>
+    <t>访问键</t>
+  </si>
+  <si>
+    <t>密码访问</t>
+  </si>
+  <si>
+    <t>管理员密码</t>
+  </si>
+  <si>
+    <t>激活的反思</t>
+  </si>
+  <si>
+    <t>禁用的反思</t>
+  </si>
+  <si>
+    <t>患者参数更新</t>
+  </si>
+  <si>
+    <t>镜像更新患者参数</t>
+  </si>
+  <si>
+    <t>患者参数复位</t>
   </si>
 </sst>
 </file>
@@ -8448,8 +8952,8 @@
   <dimension ref="A1:P242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69:XFD81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11303,108 +11807,654 @@
       </c>
     </row>
     <row r="68" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>2657</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>2660</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="C69" s="4" t="s">
+        <v>2825</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>2824</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>2838</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>2683</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>2799</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>2693</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>2704</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>2786</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>2773</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>2715</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>2761</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>2734</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>2735</v>
+      </c>
+      <c r="P69" s="4" t="s">
+        <v>2747</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>2663</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="4" t="s">
         <v>2666</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="C70" s="4" t="s">
+        <v>2826</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>2812</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>2839</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>2666</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>2800</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>2694</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>2705</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>2787</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>2774</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>2716</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>2762</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>2694</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>2736</v>
+      </c>
+      <c r="P70" s="4" t="s">
+        <v>2748</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>2664</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>2665</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="C71" s="4" t="s">
+        <v>2827</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>2813</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>2840</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>2801</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>1193</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>2788</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>2775</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>2717</v>
+      </c>
+      <c r="M71" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>1191</v>
+      </c>
+      <c r="O71" s="4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="P71" s="4" t="s">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>2658</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
         <v>2661</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="C72" s="4" t="s">
+        <v>2828</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>2814</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>2841</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>2661</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>2802</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>2695</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>2706</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>2789</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>2776</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>2661</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>2763</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>2695</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>2737</v>
+      </c>
+      <c r="P72" s="4" t="s">
+        <v>2760</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>2659</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>2662</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="C73" s="4" t="s">
+        <v>2829</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>2815</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>2842</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>2684</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>2803</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>2696</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>2662</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>2790</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>2777</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>2696</v>
+      </c>
+      <c r="M73" s="4" t="s">
+        <v>2764</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>2696</v>
+      </c>
+      <c r="O73" s="4" t="s">
+        <v>2738</v>
+      </c>
+      <c r="P73" s="4" t="s">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>2667</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="4" t="s">
         <v>2670</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="C74" s="4" t="s">
+        <v>2830</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>2816</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>2843</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>2685</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>2804</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>2697</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>2707</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>2791</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>2778</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>2718</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>2765</v>
+      </c>
+      <c r="N74" s="4" t="s">
+        <v>2726</v>
+      </c>
+      <c r="O74" s="4" t="s">
+        <v>2739</v>
+      </c>
+      <c r="P74" s="4" t="s">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>2668</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="4" t="s">
         <v>2671</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="C75" s="4" t="s">
+        <v>2831</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>2817</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>2844</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>2686</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>2805</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>2698</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>2708</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>2792</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>2779</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>2719</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>2766</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>2727</v>
+      </c>
+      <c r="O75" s="4" t="s">
+        <v>2740</v>
+      </c>
+      <c r="P75" s="4" t="s">
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>2669</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>2672</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="C76" s="4" t="s">
+        <v>2832</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>2818</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>2845</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>2687</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>2806</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>2759</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>2709</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>2793</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>2780</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>2720</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>2767</v>
+      </c>
+      <c r="N76" s="4" t="s">
+        <v>2728</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>2741</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>2673</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>2674</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="C77" s="4" t="s">
+        <v>2833</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>2819</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>2846</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>2688</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>2807</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>2699</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>2714</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>2794</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>2781</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>2725</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>2768</v>
+      </c>
+      <c r="N77" s="4" t="s">
+        <v>2729</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>2742</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>2752</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>2675</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
         <v>2676</v>
       </c>
-    </row>
-    <row r="79" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="C78" s="4" t="s">
+        <v>2834</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>2820</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>2847</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>2692</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>2808</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>2700</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>2713</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>2795</v>
+      </c>
+      <c r="K78" s="4" t="s">
+        <v>2782</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>2724</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>2769</v>
+      </c>
+      <c r="N78" s="4" t="s">
+        <v>2730</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>2743</v>
+      </c>
+      <c r="P78" s="4" t="s">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>2677</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>2679</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="C79" s="4" t="s">
+        <v>2835</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>2821</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>2848</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>2689</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>2809</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>2701</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>2710</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>2796</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>2783</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>2722</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>2770</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>2731</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>2744</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>2755</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>2678</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>2680</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="C80" s="4" t="s">
+        <v>2836</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>2822</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>2849</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>2690</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>2810</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>2703</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>2712</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>2797</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>2784</v>
+      </c>
+      <c r="L80" s="4" t="s">
+        <v>2723</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>2771</v>
+      </c>
+      <c r="N80" s="4" t="s">
+        <v>2732</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>2745</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>2681</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>2682</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>2837</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>2823</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>2850</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>2691</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>2811</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>2702</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>2711</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>2798</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>2785</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>2721</v>
+      </c>
+      <c r="M81" s="4" t="s">
+        <v>2772</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>2733</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>2746</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>2754</v>
       </c>
     </row>
     <row r="82" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>